<commit_message>
ajout définition élément location (#28)
ajout définition élément location 7f901822184ad84e0e2c288efdc568a522c04d0d
</commit_message>
<xml_diff>
--- a/ig/main/StructureDefinition-eclaire-researchstudy.xlsx
+++ b/ig/main/StructureDefinition-eclaire-researchstudy.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-07-27T08:05:38+00:00</t>
+    <t>2023-07-27T08:46:09+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -1094,7 +1094,7 @@
     <t>ResearchStudy.location</t>
   </si>
   <si>
-    <t>Geographic region(s) for study</t>
+    <t>Pays de recrutement / Countries of Recruitment</t>
   </si>
   <si>
     <t>Indicates a country, state or other region where the study is taking place.</t>
@@ -1194,7 +1194,7 @@
     <t>ResearchStudy.sponsor</t>
   </si>
   <si>
-    <t>promoteur / primary Sponsor</t>
+    <t>Promoteur / primary Sponsor</t>
   </si>
   <si>
     <t>An organization that initiates the investigation and is legally responsible for the study.</t>

</xml_diff>

<commit_message>
extension contact spécifique au site (#36)
* ajout extension ECLAIRESiteContactName

* add profil location et extension ECLAIRESiteContactName

add profil location et extension ECLAIRESiteContactName dans location
+ Ajout MS pour les éléments profilés

* typo

* correction extension dans profil location

correction erreur sur l'extension

* changement type extension

string => HumanName 5b2c74f2fc2d6b9750669722b03d9bf42d88cea1
</commit_message>
<xml_diff>
--- a/ig/main/StructureDefinition-eclaire-researchstudy.xlsx
+++ b/ig/main/StructureDefinition-eclaire-researchstudy.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-07-27T15:15:25+00:00</t>
+    <t>2023-07-28T08:09:21+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -75,7 +75,7 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Profil pour le projet ECLAIRE</t>
+    <t>Profil de ResearchStudy pour le projet ECLAIRE</t>
   </si>
   <si>
     <t>Purpose</t>
@@ -2752,7 +2752,7 @@
         <v>46</v>
       </c>
       <c r="H9" t="s" s="2">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="I9" t="s" s="2">
         <v>37</v>
@@ -2869,7 +2869,7 @@
         <v>46</v>
       </c>
       <c r="H10" t="s" s="2">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="I10" t="s" s="2">
         <v>37</v>
@@ -2986,7 +2986,7 @@
         <v>46</v>
       </c>
       <c r="H11" t="s" s="2">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="I11" t="s" s="2">
         <v>37</v>
@@ -3103,7 +3103,7 @@
         <v>46</v>
       </c>
       <c r="H12" t="s" s="2">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="I12" t="s" s="2">
         <v>37</v>
@@ -3220,7 +3220,7 @@
         <v>36</v>
       </c>
       <c r="H13" t="s" s="2">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="I13" t="s" s="2">
         <v>37</v>
@@ -3337,7 +3337,7 @@
         <v>36</v>
       </c>
       <c r="H14" t="s" s="2">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="I14" t="s" s="2">
         <v>37</v>
@@ -5806,7 +5806,7 @@
         <v>46</v>
       </c>
       <c r="H35" t="s" s="2">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="I35" t="s" s="2">
         <v>37</v>
@@ -6159,7 +6159,7 @@
         <v>46</v>
       </c>
       <c r="H38" t="s" s="2">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="I38" t="s" s="2">
         <v>47</v>
@@ -6393,7 +6393,7 @@
         <v>46</v>
       </c>
       <c r="H40" t="s" s="2">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="I40" t="s" s="2">
         <v>37</v>
@@ -6510,7 +6510,7 @@
         <v>36</v>
       </c>
       <c r="H41" t="s" s="2">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="I41" t="s" s="2">
         <v>37</v>
@@ -6744,7 +6744,7 @@
         <v>36</v>
       </c>
       <c r="H43" t="s" s="2">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="I43" t="s" s="2">
         <v>37</v>
@@ -6861,7 +6861,7 @@
         <v>36</v>
       </c>
       <c r="H44" t="s" s="2">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="I44" t="s" s="2">
         <v>37</v>
@@ -7210,7 +7210,7 @@
         <v>46</v>
       </c>
       <c r="H47" t="s" s="2">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="I47" t="s" s="2">
         <v>37</v>
@@ -7791,7 +7791,7 @@
         <v>36</v>
       </c>
       <c r="H52" t="s" s="2">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="I52" t="s" s="2">
         <v>37</v>
@@ -7908,7 +7908,7 @@
         <v>46</v>
       </c>
       <c r="H53" t="s" s="2">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="I53" t="s" s="2">
         <v>37</v>
@@ -8025,7 +8025,7 @@
         <v>36</v>
       </c>
       <c r="H54" t="s" s="2">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="I54" t="s" s="2">
         <v>37</v>
@@ -8259,7 +8259,7 @@
         <v>46</v>
       </c>
       <c r="H56" t="s" s="2">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="I56" t="s" s="2">
         <v>37</v>
@@ -8493,7 +8493,7 @@
         <v>36</v>
       </c>
       <c r="H58" t="s" s="2">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="I58" t="s" s="2">
         <v>37</v>

</xml_diff>

<commit_message>
ajout valeur phase de lessai (#39)
* creation VS pour phase

* test correction

* correctif

* typo

* correctif binding

* Update EclaireStudyPhaseVS.fsh 9bb1f32f0978b9cf152bbd411d8f3028f06733ba
</commit_message>
<xml_diff>
--- a/ig/main/StructureDefinition-eclaire-researchstudy.xlsx
+++ b/ig/main/StructureDefinition-eclaire-researchstudy.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2737" uniqueCount="457">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2736" uniqueCount="456">
   <si>
     <t>Property</t>
   </si>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-07-28T08:09:21+00:00</t>
+    <t>2023-07-28T15:45:52+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -894,28 +894,25 @@
     <t>The stage in the progression of a therapy from initial experimental use in humans in clinical trials to post-market evaluation.</t>
   </si>
   <si>
+    <t>https://interop.esante.gouv.fr/ig/fhir/eclaire/ValueSet/eclaire-study-phase-vs</t>
+  </si>
+  <si>
+    <t>StudyProtocolVersion.phaseCode</t>
+  </si>
+  <si>
+    <t>Study Phase</t>
+  </si>
+  <si>
+    <t>ResearchStudy.category</t>
+  </si>
+  <si>
+    <t>Type d'essai  / Study type : type of study</t>
+  </si>
+  <si>
+    <t>Codes categorizing the type of study such as investigational vs. observational, type of blinding, type of randomization, safety vs. efficacy, etc.</t>
+  </si>
+  <si>
     <t>example</t>
-  </si>
-  <si>
-    <t>Codes for the stage in the progression of a therapy from initial experimental use in humans in clinical trials to post-market evaluation.</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/ValueSet/research-study-phase</t>
-  </si>
-  <si>
-    <t>StudyProtocolVersion.phaseCode</t>
-  </si>
-  <si>
-    <t>Study Phase</t>
-  </si>
-  <si>
-    <t>ResearchStudy.category</t>
-  </si>
-  <si>
-    <t>Type d'essai  / Study type : type of study</t>
-  </si>
-  <si>
-    <t>Codes categorizing the type of study such as investigational vs. observational, type of blinding, type of randomization, safety vs. efficacy, etc.</t>
   </si>
   <si>
     <t>Codes that describe the type of research study.  E.g. Study phase, Interventional/Observational, blinding type, etc.</t>
@@ -1778,8 +1775,8 @@
     <col min="22" max="22" width="1.04296875" customWidth="true" bestFit="true"/>
     <col min="23" max="23" width="1.04296875" customWidth="true" bestFit="true"/>
     <col min="24" max="24" width="10.53125" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="124.69140625" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="54.97265625" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="106.69140625" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="71.046875" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="1.04296875" customWidth="true" bestFit="true"/>
     <col min="28" max="28" width="11.08203125" customWidth="true" bestFit="true"/>
     <col min="29" max="29" width="52.18359375" customWidth="true" bestFit="true"/>
@@ -6437,13 +6434,11 @@
         <v>37</v>
       </c>
       <c r="X40" t="s" s="2">
+        <v>182</v>
+      </c>
+      <c r="Y40" s="2"/>
+      <c r="Z40" t="s" s="2">
         <v>280</v>
-      </c>
-      <c r="Y40" t="s" s="2">
-        <v>281</v>
-      </c>
-      <c r="Z40" t="s" s="2">
-        <v>282</v>
       </c>
       <c r="AA40" t="s" s="2">
         <v>37</v>
@@ -6476,7 +6471,7 @@
         <v>59</v>
       </c>
       <c r="AK40" t="s" s="2">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="AL40" t="s" s="2">
         <v>275</v>
@@ -6485,7 +6480,7 @@
         <v>276</v>
       </c>
       <c r="AN40" t="s" s="2">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="AO40" t="s" s="2">
         <v>37</v>
@@ -6493,10 +6488,10 @@
     </row>
     <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B41" t="s" s="2">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C41" s="2"/>
       <c r="D41" t="s" s="2">
@@ -6522,10 +6517,10 @@
         <v>177</v>
       </c>
       <c r="L41" t="s" s="2">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="M41" t="s" s="2">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="N41" t="s" s="2">
         <v>271</v>
@@ -6554,10 +6549,10 @@
         <v>37</v>
       </c>
       <c r="X41" t="s" s="2">
-        <v>280</v>
+        <v>286</v>
       </c>
       <c r="Y41" t="s" s="2">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="Z41" t="s" s="2">
         <v>37</v>
@@ -6578,7 +6573,7 @@
         <v>37</v>
       </c>
       <c r="AF41" t="s" s="2">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="AG41" t="s" s="2">
         <v>35</v>
@@ -6593,7 +6588,7 @@
         <v>59</v>
       </c>
       <c r="AK41" t="s" s="2">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="AL41" t="s" s="2">
         <v>275</v>
@@ -6602,7 +6597,7 @@
         <v>276</v>
       </c>
       <c r="AN41" t="s" s="2">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="AO41" t="s" s="2">
         <v>37</v>
@@ -6610,10 +6605,10 @@
     </row>
     <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B42" t="s" s="2">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C42" s="2"/>
       <c r="D42" t="s" s="2">
@@ -6639,10 +6634,10 @@
         <v>177</v>
       </c>
       <c r="L42" t="s" s="2">
+        <v>291</v>
+      </c>
+      <c r="M42" t="s" s="2">
         <v>292</v>
-      </c>
-      <c r="M42" t="s" s="2">
-        <v>293</v>
       </c>
       <c r="N42" t="s" s="2">
         <v>271</v>
@@ -6671,10 +6666,10 @@
         <v>37</v>
       </c>
       <c r="X42" t="s" s="2">
-        <v>280</v>
+        <v>286</v>
       </c>
       <c r="Y42" t="s" s="2">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="Z42" t="s" s="2">
         <v>37</v>
@@ -6695,7 +6690,7 @@
         <v>37</v>
       </c>
       <c r="AF42" t="s" s="2">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="AG42" t="s" s="2">
         <v>35</v>
@@ -6710,7 +6705,7 @@
         <v>59</v>
       </c>
       <c r="AK42" t="s" s="2">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="AL42" t="s" s="2">
         <v>275</v>
@@ -6719,18 +6714,18 @@
         <v>276</v>
       </c>
       <c r="AN42" t="s" s="2">
+        <v>295</v>
+      </c>
+      <c r="AO42" t="s" s="2">
         <v>296</v>
-      </c>
-      <c r="AO42" t="s" s="2">
-        <v>297</v>
       </c>
     </row>
     <row r="43" hidden="true">
       <c r="A43" t="s" s="2">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B43" t="s" s="2">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C43" s="2"/>
       <c r="D43" t="s" s="2">
@@ -6756,10 +6751,10 @@
         <v>177</v>
       </c>
       <c r="L43" t="s" s="2">
+        <v>298</v>
+      </c>
+      <c r="M43" t="s" s="2">
         <v>299</v>
-      </c>
-      <c r="M43" t="s" s="2">
-        <v>300</v>
       </c>
       <c r="N43" t="s" s="2">
         <v>271</v>
@@ -6788,14 +6783,14 @@
         <v>37</v>
       </c>
       <c r="X43" t="s" s="2">
-        <v>280</v>
+        <v>286</v>
       </c>
       <c r="Y43" t="s" s="2">
+        <v>300</v>
+      </c>
+      <c r="Z43" t="s" s="2">
         <v>301</v>
       </c>
-      <c r="Z43" t="s" s="2">
-        <v>302</v>
-      </c>
       <c r="AA43" t="s" s="2">
         <v>37</v>
       </c>
@@ -6812,7 +6807,7 @@
         <v>37</v>
       </c>
       <c r="AF43" t="s" s="2">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="AG43" t="s" s="2">
         <v>35</v>
@@ -6827,7 +6822,7 @@
         <v>59</v>
       </c>
       <c r="AK43" t="s" s="2">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="AL43" t="s" s="2">
         <v>275</v>
@@ -6836,18 +6831,18 @@
         <v>276</v>
       </c>
       <c r="AN43" t="s" s="2">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="AO43" t="s" s="2">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B44" t="s" s="2">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C44" s="2"/>
       <c r="D44" t="s" s="2">
@@ -6870,13 +6865,13 @@
         <v>47</v>
       </c>
       <c r="K44" t="s" s="2">
+        <v>305</v>
+      </c>
+      <c r="L44" t="s" s="2">
         <v>306</v>
       </c>
-      <c r="L44" t="s" s="2">
+      <c r="M44" t="s" s="2">
         <v>307</v>
-      </c>
-      <c r="M44" t="s" s="2">
-        <v>308</v>
       </c>
       <c r="N44" s="2"/>
       <c r="O44" s="2"/>
@@ -6927,7 +6922,7 @@
         <v>37</v>
       </c>
       <c r="AF44" t="s" s="2">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="AG44" t="s" s="2">
         <v>35</v>
@@ -6942,7 +6937,7 @@
         <v>59</v>
       </c>
       <c r="AK44" t="s" s="2">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="AL44" t="s" s="2">
         <v>37</v>
@@ -6951,7 +6946,7 @@
         <v>67</v>
       </c>
       <c r="AN44" t="s" s="2">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="AO44" t="s" s="2">
         <v>37</v>
@@ -6959,10 +6954,10 @@
     </row>
     <row r="45" hidden="true">
       <c r="A45" t="s" s="2">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B45" t="s" s="2">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C45" s="2"/>
       <c r="D45" t="s" s="2">
@@ -7074,10 +7069,10 @@
     </row>
     <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B46" t="s" s="2">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C46" s="2"/>
       <c r="D46" t="s" s="2">
@@ -7191,13 +7186,13 @@
     </row>
     <row r="47" hidden="true">
       <c r="A47" t="s" s="2">
+        <v>312</v>
+      </c>
+      <c r="B47" t="s" s="2">
+        <v>311</v>
+      </c>
+      <c r="C47" t="s" s="2">
         <v>313</v>
-      </c>
-      <c r="B47" t="s" s="2">
-        <v>312</v>
-      </c>
-      <c r="C47" t="s" s="2">
-        <v>314</v>
       </c>
       <c r="D47" t="s" s="2">
         <v>37</v>
@@ -7219,13 +7214,13 @@
         <v>37</v>
       </c>
       <c r="K47" t="s" s="2">
+        <v>314</v>
+      </c>
+      <c r="L47" t="s" s="2">
         <v>315</v>
       </c>
-      <c r="L47" t="s" s="2">
+      <c r="M47" t="s" s="2">
         <v>316</v>
-      </c>
-      <c r="M47" t="s" s="2">
-        <v>317</v>
       </c>
       <c r="N47" s="2"/>
       <c r="O47" s="2"/>
@@ -7308,10 +7303,10 @@
     </row>
     <row r="48" hidden="true">
       <c r="A48" t="s" s="2">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B48" t="s" s="2">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C48" s="2"/>
       <c r="D48" t="s" s="2">
@@ -7337,13 +7332,13 @@
         <v>155</v>
       </c>
       <c r="L48" t="s" s="2">
+        <v>318</v>
+      </c>
+      <c r="M48" t="s" s="2">
         <v>319</v>
       </c>
-      <c r="M48" t="s" s="2">
+      <c r="N48" t="s" s="2">
         <v>320</v>
-      </c>
-      <c r="N48" t="s" s="2">
-        <v>321</v>
       </c>
       <c r="O48" s="2"/>
       <c r="P48" t="s" s="2">
@@ -7393,7 +7388,7 @@
         <v>37</v>
       </c>
       <c r="AF48" t="s" s="2">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="AG48" t="s" s="2">
         <v>35</v>
@@ -7425,10 +7420,10 @@
     </row>
     <row r="49" hidden="true">
       <c r="A49" t="s" s="2">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B49" t="s" s="2">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C49" s="2"/>
       <c r="D49" t="s" s="2">
@@ -7451,13 +7446,13 @@
         <v>47</v>
       </c>
       <c r="K49" t="s" s="2">
+        <v>323</v>
+      </c>
+      <c r="L49" t="s" s="2">
         <v>324</v>
       </c>
-      <c r="L49" t="s" s="2">
+      <c r="M49" t="s" s="2">
         <v>325</v>
-      </c>
-      <c r="M49" t="s" s="2">
-        <v>326</v>
       </c>
       <c r="N49" s="2"/>
       <c r="O49" s="2"/>
@@ -7508,7 +7503,7 @@
         <v>37</v>
       </c>
       <c r="AF49" t="s" s="2">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="AG49" t="s" s="2">
         <v>35</v>
@@ -7520,16 +7515,16 @@
         <v>58</v>
       </c>
       <c r="AJ49" t="s" s="2">
+        <v>327</v>
+      </c>
+      <c r="AK49" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AL49" t="s" s="2">
         <v>328</v>
       </c>
-      <c r="AK49" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AL49" t="s" s="2">
+      <c r="AM49" t="s" s="2">
         <v>329</v>
-      </c>
-      <c r="AM49" t="s" s="2">
-        <v>330</v>
       </c>
       <c r="AN49" t="s" s="2">
         <v>37</v>
@@ -7540,10 +7535,10 @@
     </row>
     <row r="50" hidden="true">
       <c r="A50" t="s" s="2">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B50" t="s" s="2">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C50" s="2"/>
       <c r="D50" t="s" s="2">
@@ -7566,16 +7561,16 @@
         <v>37</v>
       </c>
       <c r="K50" t="s" s="2">
+        <v>331</v>
+      </c>
+      <c r="L50" t="s" s="2">
         <v>332</v>
       </c>
-      <c r="L50" t="s" s="2">
+      <c r="M50" t="s" s="2">
         <v>333</v>
       </c>
-      <c r="M50" t="s" s="2">
+      <c r="N50" t="s" s="2">
         <v>334</v>
-      </c>
-      <c r="N50" t="s" s="2">
-        <v>335</v>
       </c>
       <c r="O50" s="2"/>
       <c r="P50" t="s" s="2">
@@ -7625,7 +7620,7 @@
         <v>37</v>
       </c>
       <c r="AF50" t="s" s="2">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="AG50" t="s" s="2">
         <v>35</v>
@@ -7640,7 +7635,7 @@
         <v>59</v>
       </c>
       <c r="AK50" t="s" s="2">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="AL50" t="s" s="2">
         <v>37</v>
@@ -7649,7 +7644,7 @@
         <v>67</v>
       </c>
       <c r="AN50" t="s" s="2">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="AO50" t="s" s="2">
         <v>37</v>
@@ -7657,10 +7652,10 @@
     </row>
     <row r="51" hidden="true">
       <c r="A51" t="s" s="2">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B51" t="s" s="2">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C51" s="2"/>
       <c r="D51" t="s" s="2">
@@ -7686,10 +7681,10 @@
         <v>177</v>
       </c>
       <c r="L51" t="s" s="2">
+        <v>338</v>
+      </c>
+      <c r="M51" t="s" s="2">
         <v>339</v>
-      </c>
-      <c r="M51" t="s" s="2">
-        <v>340</v>
       </c>
       <c r="N51" t="s" s="2">
         <v>271</v>
@@ -7718,10 +7713,10 @@
         <v>37</v>
       </c>
       <c r="X51" t="s" s="2">
-        <v>280</v>
+        <v>286</v>
       </c>
       <c r="Y51" t="s" s="2">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="Z51" t="s" s="2">
         <v>37</v>
@@ -7742,7 +7737,7 @@
         <v>37</v>
       </c>
       <c r="AF51" t="s" s="2">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="AG51" t="s" s="2">
         <v>35</v>
@@ -7757,7 +7752,7 @@
         <v>59</v>
       </c>
       <c r="AK51" t="s" s="2">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="AL51" t="s" s="2">
         <v>275</v>
@@ -7766,7 +7761,7 @@
         <v>276</v>
       </c>
       <c r="AN51" t="s" s="2">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="AO51" t="s" s="2">
         <v>37</v>
@@ -7774,10 +7769,10 @@
     </row>
     <row r="52" hidden="true">
       <c r="A52" t="s" s="2">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B52" t="s" s="2">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C52" s="2"/>
       <c r="D52" t="s" s="2">
@@ -7803,10 +7798,10 @@
         <v>177</v>
       </c>
       <c r="L52" t="s" s="2">
+        <v>344</v>
+      </c>
+      <c r="M52" t="s" s="2">
         <v>345</v>
-      </c>
-      <c r="M52" t="s" s="2">
-        <v>346</v>
       </c>
       <c r="N52" t="s" s="2">
         <v>271</v>
@@ -7838,11 +7833,11 @@
         <v>182</v>
       </c>
       <c r="Y52" t="s" s="2">
+        <v>346</v>
+      </c>
+      <c r="Z52" t="s" s="2">
         <v>347</v>
       </c>
-      <c r="Z52" t="s" s="2">
-        <v>348</v>
-      </c>
       <c r="AA52" t="s" s="2">
         <v>37</v>
       </c>
@@ -7859,7 +7854,7 @@
         <v>37</v>
       </c>
       <c r="AF52" t="s" s="2">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="AG52" t="s" s="2">
         <v>35</v>
@@ -7874,7 +7869,7 @@
         <v>59</v>
       </c>
       <c r="AK52" t="s" s="2">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="AL52" t="s" s="2">
         <v>275</v>
@@ -7891,10 +7886,10 @@
     </row>
     <row r="53" hidden="true">
       <c r="A53" t="s" s="2">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B53" t="s" s="2">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C53" s="2"/>
       <c r="D53" t="s" s="2">
@@ -7917,16 +7912,16 @@
         <v>37</v>
       </c>
       <c r="K53" t="s" s="2">
+        <v>350</v>
+      </c>
+      <c r="L53" t="s" s="2">
         <v>351</v>
       </c>
-      <c r="L53" t="s" s="2">
+      <c r="M53" t="s" s="2">
         <v>352</v>
       </c>
-      <c r="M53" t="s" s="2">
+      <c r="N53" t="s" s="2">
         <v>353</v>
-      </c>
-      <c r="N53" t="s" s="2">
-        <v>354</v>
       </c>
       <c r="O53" s="2"/>
       <c r="P53" t="s" s="2">
@@ -7976,7 +7971,7 @@
         <v>37</v>
       </c>
       <c r="AF53" t="s" s="2">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="AG53" t="s" s="2">
         <v>35</v>
@@ -7991,7 +7986,7 @@
         <v>59</v>
       </c>
       <c r="AK53" t="s" s="2">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="AL53" t="s" s="2">
         <v>37</v>
@@ -8000,7 +7995,7 @@
         <v>67</v>
       </c>
       <c r="AN53" t="s" s="2">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="AO53" t="s" s="2">
         <v>37</v>
@@ -8008,14 +8003,14 @@
     </row>
     <row r="54" hidden="true">
       <c r="A54" t="s" s="2">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B54" t="s" s="2">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C54" s="2"/>
       <c r="D54" t="s" s="2">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="E54" s="2"/>
       <c r="F54" t="s" s="2">
@@ -8034,16 +8029,16 @@
         <v>47</v>
       </c>
       <c r="K54" t="s" s="2">
+        <v>358</v>
+      </c>
+      <c r="L54" t="s" s="2">
         <v>359</v>
       </c>
-      <c r="L54" t="s" s="2">
+      <c r="M54" t="s" s="2">
         <v>360</v>
       </c>
-      <c r="M54" t="s" s="2">
+      <c r="N54" t="s" s="2">
         <v>361</v>
-      </c>
-      <c r="N54" t="s" s="2">
-        <v>362</v>
       </c>
       <c r="O54" s="2"/>
       <c r="P54" t="s" s="2">
@@ -8093,7 +8088,7 @@
         <v>37</v>
       </c>
       <c r="AF54" t="s" s="2">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="AG54" t="s" s="2">
         <v>35</v>
@@ -8108,31 +8103,31 @@
         <v>223</v>
       </c>
       <c r="AK54" t="s" s="2">
+        <v>362</v>
+      </c>
+      <c r="AL54" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AM54" t="s" s="2">
         <v>363</v>
       </c>
-      <c r="AL54" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AM54" t="s" s="2">
+      <c r="AN54" t="s" s="2">
         <v>364</v>
       </c>
-      <c r="AN54" t="s" s="2">
+      <c r="AO54" t="s" s="2">
         <v>365</v>
-      </c>
-      <c r="AO54" t="s" s="2">
-        <v>366</v>
       </c>
     </row>
     <row r="55" hidden="true">
       <c r="A55" t="s" s="2">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B55" t="s" s="2">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C55" s="2"/>
       <c r="D55" t="s" s="2">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="E55" s="2"/>
       <c r="F55" t="s" s="2">
@@ -8154,10 +8149,10 @@
         <v>208</v>
       </c>
       <c r="L55" t="s" s="2">
+        <v>368</v>
+      </c>
+      <c r="M55" t="s" s="2">
         <v>369</v>
-      </c>
-      <c r="M55" t="s" s="2">
-        <v>370</v>
       </c>
       <c r="N55" t="s" s="2">
         <v>211</v>
@@ -8210,7 +8205,7 @@
         <v>37</v>
       </c>
       <c r="AF55" t="s" s="2">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="AG55" t="s" s="2">
         <v>35</v>
@@ -8225,27 +8220,27 @@
         <v>213</v>
       </c>
       <c r="AK55" t="s" s="2">
+        <v>370</v>
+      </c>
+      <c r="AL55" t="s" s="2">
         <v>371</v>
       </c>
-      <c r="AL55" t="s" s="2">
+      <c r="AM55" t="s" s="2">
         <v>372</v>
       </c>
-      <c r="AM55" t="s" s="2">
+      <c r="AN55" t="s" s="2">
         <v>373</v>
       </c>
-      <c r="AN55" t="s" s="2">
+      <c r="AO55" t="s" s="2">
         <v>374</v>
-      </c>
-      <c r="AO55" t="s" s="2">
-        <v>375</v>
       </c>
     </row>
     <row r="56" hidden="true">
       <c r="A56" t="s" s="2">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B56" t="s" s="2">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C56" s="2"/>
       <c r="D56" t="s" s="2">
@@ -8271,10 +8266,10 @@
         <v>218</v>
       </c>
       <c r="L56" t="s" s="2">
+        <v>376</v>
+      </c>
+      <c r="M56" t="s" s="2">
         <v>377</v>
-      </c>
-      <c r="M56" t="s" s="2">
-        <v>378</v>
       </c>
       <c r="N56" t="s" s="2">
         <v>248</v>
@@ -8327,7 +8322,7 @@
         <v>37</v>
       </c>
       <c r="AF56" t="s" s="2">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="AG56" t="s" s="2">
         <v>35</v>
@@ -8342,27 +8337,27 @@
         <v>223</v>
       </c>
       <c r="AK56" t="s" s="2">
+        <v>378</v>
+      </c>
+      <c r="AL56" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AM56" t="s" s="2">
         <v>379</v>
       </c>
-      <c r="AL56" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AM56" t="s" s="2">
+      <c r="AN56" t="s" s="2">
         <v>380</v>
       </c>
-      <c r="AN56" t="s" s="2">
+      <c r="AO56" t="s" s="2">
         <v>381</v>
-      </c>
-      <c r="AO56" t="s" s="2">
-        <v>382</v>
       </c>
     </row>
     <row r="57" hidden="true">
       <c r="A57" t="s" s="2">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B57" t="s" s="2">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C57" s="2"/>
       <c r="D57" t="s" s="2">
@@ -8385,13 +8380,13 @@
         <v>47</v>
       </c>
       <c r="K57" t="s" s="2">
+        <v>383</v>
+      </c>
+      <c r="L57" t="s" s="2">
         <v>384</v>
       </c>
-      <c r="L57" t="s" s="2">
+      <c r="M57" t="s" s="2">
         <v>385</v>
-      </c>
-      <c r="M57" t="s" s="2">
-        <v>386</v>
       </c>
       <c r="N57" t="s" s="2">
         <v>248</v>
@@ -8444,7 +8439,7 @@
         <v>37</v>
       </c>
       <c r="AF57" t="s" s="2">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="AG57" t="s" s="2">
         <v>35</v>
@@ -8459,27 +8454,27 @@
         <v>223</v>
       </c>
       <c r="AK57" t="s" s="2">
+        <v>386</v>
+      </c>
+      <c r="AL57" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AM57" t="s" s="2">
         <v>387</v>
       </c>
-      <c r="AL57" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AM57" t="s" s="2">
+      <c r="AN57" t="s" s="2">
         <v>388</v>
       </c>
-      <c r="AN57" t="s" s="2">
-        <v>389</v>
-      </c>
       <c r="AO57" t="s" s="2">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="58" hidden="true">
       <c r="A58" t="s" s="2">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B58" t="s" s="2">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="C58" s="2"/>
       <c r="D58" t="s" s="2">
@@ -8502,13 +8497,13 @@
         <v>47</v>
       </c>
       <c r="K58" t="s" s="2">
+        <v>390</v>
+      </c>
+      <c r="L58" t="s" s="2">
         <v>391</v>
       </c>
-      <c r="L58" t="s" s="2">
+      <c r="M58" t="s" s="2">
         <v>392</v>
-      </c>
-      <c r="M58" t="s" s="2">
-        <v>393</v>
       </c>
       <c r="N58" t="s" s="2">
         <v>248</v>
@@ -8561,7 +8556,7 @@
         <v>37</v>
       </c>
       <c r="AF58" t="s" s="2">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="AG58" t="s" s="2">
         <v>35</v>
@@ -8576,27 +8571,27 @@
         <v>223</v>
       </c>
       <c r="AK58" t="s" s="2">
+        <v>393</v>
+      </c>
+      <c r="AL58" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AM58" t="s" s="2">
+        <v>387</v>
+      </c>
+      <c r="AN58" t="s" s="2">
         <v>394</v>
       </c>
-      <c r="AL58" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AM58" t="s" s="2">
-        <v>388</v>
-      </c>
-      <c r="AN58" t="s" s="2">
+      <c r="AO58" t="s" s="2">
         <v>395</v>
-      </c>
-      <c r="AO58" t="s" s="2">
-        <v>396</v>
       </c>
     </row>
     <row r="59" hidden="true">
       <c r="A59" t="s" s="2">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B59" t="s" s="2">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C59" s="2"/>
       <c r="D59" t="s" s="2">
@@ -8622,10 +8617,10 @@
         <v>177</v>
       </c>
       <c r="L59" t="s" s="2">
+        <v>397</v>
+      </c>
+      <c r="M59" t="s" s="2">
         <v>398</v>
-      </c>
-      <c r="M59" t="s" s="2">
-        <v>399</v>
       </c>
       <c r="N59" t="s" s="2">
         <v>271</v>
@@ -8654,14 +8649,14 @@
         <v>37</v>
       </c>
       <c r="X59" t="s" s="2">
-        <v>280</v>
+        <v>286</v>
       </c>
       <c r="Y59" t="s" s="2">
+        <v>399</v>
+      </c>
+      <c r="Z59" t="s" s="2">
         <v>400</v>
       </c>
-      <c r="Z59" t="s" s="2">
-        <v>401</v>
-      </c>
       <c r="AA59" t="s" s="2">
         <v>37</v>
       </c>
@@ -8678,7 +8673,7 @@
         <v>37</v>
       </c>
       <c r="AF59" t="s" s="2">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="AG59" t="s" s="2">
         <v>35</v>
@@ -8693,7 +8688,7 @@
         <v>59</v>
       </c>
       <c r="AK59" t="s" s="2">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="AL59" t="s" s="2">
         <v>275</v>
@@ -8702,18 +8697,18 @@
         <v>276</v>
       </c>
       <c r="AN59" t="s" s="2">
+        <v>402</v>
+      </c>
+      <c r="AO59" t="s" s="2">
         <v>403</v>
-      </c>
-      <c r="AO59" t="s" s="2">
-        <v>404</v>
       </c>
     </row>
     <row r="60" hidden="true">
       <c r="A60" t="s" s="2">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B60" t="s" s="2">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="C60" s="2"/>
       <c r="D60" t="s" s="2">
@@ -8736,16 +8731,16 @@
         <v>37</v>
       </c>
       <c r="K60" t="s" s="2">
+        <v>405</v>
+      </c>
+      <c r="L60" t="s" s="2">
         <v>406</v>
       </c>
-      <c r="L60" t="s" s="2">
+      <c r="M60" t="s" s="2">
         <v>407</v>
       </c>
-      <c r="M60" t="s" s="2">
+      <c r="N60" t="s" s="2">
         <v>408</v>
-      </c>
-      <c r="N60" t="s" s="2">
-        <v>409</v>
       </c>
       <c r="O60" s="2"/>
       <c r="P60" t="s" s="2">
@@ -8795,7 +8790,7 @@
         <v>37</v>
       </c>
       <c r="AF60" t="s" s="2">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="AG60" t="s" s="2">
         <v>35</v>
@@ -8810,13 +8805,13 @@
         <v>59</v>
       </c>
       <c r="AK60" t="s" s="2">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="AL60" t="s" s="2">
         <v>60</v>
       </c>
       <c r="AM60" t="s" s="2">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="AN60" t="s" s="2">
         <v>37</v>
@@ -8827,10 +8822,10 @@
     </row>
     <row r="61" hidden="true">
       <c r="A61" t="s" s="2">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B61" t="s" s="2">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C61" s="2"/>
       <c r="D61" t="s" s="2">
@@ -8853,13 +8848,13 @@
         <v>37</v>
       </c>
       <c r="K61" t="s" s="2">
+        <v>412</v>
+      </c>
+      <c r="L61" t="s" s="2">
         <v>413</v>
       </c>
-      <c r="L61" t="s" s="2">
+      <c r="M61" t="s" s="2">
         <v>414</v>
-      </c>
-      <c r="M61" t="s" s="2">
-        <v>415</v>
       </c>
       <c r="N61" s="2"/>
       <c r="O61" s="2"/>
@@ -8910,7 +8905,7 @@
         <v>37</v>
       </c>
       <c r="AF61" t="s" s="2">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="AG61" t="s" s="2">
         <v>35</v>
@@ -8925,7 +8920,7 @@
         <v>59</v>
       </c>
       <c r="AK61" t="s" s="2">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="AL61" t="s" s="2">
         <v>37</v>
@@ -8934,7 +8929,7 @@
         <v>67</v>
       </c>
       <c r="AN61" t="s" s="2">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="AO61" t="s" s="2">
         <v>37</v>
@@ -8942,10 +8937,10 @@
     </row>
     <row r="62" hidden="true">
       <c r="A62" t="s" s="2">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B62" t="s" s="2">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="C62" s="2"/>
       <c r="D62" t="s" s="2">
@@ -9057,10 +9052,10 @@
     </row>
     <row r="63" hidden="true">
       <c r="A63" t="s" s="2">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B63" t="s" s="2">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C63" s="2"/>
       <c r="D63" t="s" s="2">
@@ -9174,14 +9169,14 @@
     </row>
     <row r="64" hidden="true">
       <c r="A64" t="s" s="2">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B64" t="s" s="2">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C64" s="2"/>
       <c r="D64" t="s" s="2">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="E64" s="2"/>
       <c r="F64" t="s" s="2">
@@ -9203,10 +9198,10 @@
         <v>94</v>
       </c>
       <c r="L64" t="s" s="2">
+        <v>421</v>
+      </c>
+      <c r="M64" t="s" s="2">
         <v>422</v>
-      </c>
-      <c r="M64" t="s" s="2">
-        <v>423</v>
       </c>
       <c r="N64" t="s" s="2">
         <v>97</v>
@@ -9261,7 +9256,7 @@
         <v>37</v>
       </c>
       <c r="AF64" t="s" s="2">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="AG64" t="s" s="2">
         <v>35</v>
@@ -9293,10 +9288,10 @@
     </row>
     <row r="65" hidden="true">
       <c r="A65" t="s" s="2">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B65" t="s" s="2">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C65" s="2"/>
       <c r="D65" t="s" s="2">
@@ -9322,10 +9317,10 @@
         <v>155</v>
       </c>
       <c r="L65" t="s" s="2">
+        <v>425</v>
+      </c>
+      <c r="M65" t="s" s="2">
         <v>426</v>
-      </c>
-      <c r="M65" t="s" s="2">
-        <v>427</v>
       </c>
       <c r="N65" t="s" s="2">
         <v>241</v>
@@ -9378,7 +9373,7 @@
         <v>37</v>
       </c>
       <c r="AF65" t="s" s="2">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="AG65" t="s" s="2">
         <v>46</v>
@@ -9393,7 +9388,7 @@
         <v>59</v>
       </c>
       <c r="AK65" t="s" s="2">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="AL65" t="s" s="2">
         <v>37</v>
@@ -9402,7 +9397,7 @@
         <v>67</v>
       </c>
       <c r="AN65" t="s" s="2">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="AO65" t="s" s="2">
         <v>37</v>
@@ -9410,10 +9405,10 @@
     </row>
     <row r="66" hidden="true">
       <c r="A66" t="s" s="2">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B66" t="s" s="2">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="C66" s="2"/>
       <c r="D66" t="s" s="2">
@@ -9439,10 +9434,10 @@
         <v>177</v>
       </c>
       <c r="L66" t="s" s="2">
+        <v>430</v>
+      </c>
+      <c r="M66" t="s" s="2">
         <v>431</v>
-      </c>
-      <c r="M66" t="s" s="2">
-        <v>432</v>
       </c>
       <c r="N66" t="s" s="2">
         <v>271</v>
@@ -9495,7 +9490,7 @@
         <v>37</v>
       </c>
       <c r="AF66" t="s" s="2">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="AG66" t="s" s="2">
         <v>35</v>
@@ -9510,7 +9505,7 @@
         <v>59</v>
       </c>
       <c r="AK66" t="s" s="2">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="AL66" t="s" s="2">
         <v>275</v>
@@ -9519,7 +9514,7 @@
         <v>276</v>
       </c>
       <c r="AN66" t="s" s="2">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="AO66" t="s" s="2">
         <v>37</v>
@@ -9527,10 +9522,10 @@
     </row>
     <row r="67" hidden="true">
       <c r="A67" t="s" s="2">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B67" t="s" s="2">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C67" s="2"/>
       <c r="D67" t="s" s="2">
@@ -9556,10 +9551,10 @@
         <v>155</v>
       </c>
       <c r="L67" t="s" s="2">
+        <v>435</v>
+      </c>
+      <c r="M67" t="s" s="2">
         <v>436</v>
-      </c>
-      <c r="M67" t="s" s="2">
-        <v>437</v>
       </c>
       <c r="N67" t="s" s="2">
         <v>241</v>
@@ -9612,7 +9607,7 @@
         <v>37</v>
       </c>
       <c r="AF67" t="s" s="2">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="AG67" t="s" s="2">
         <v>35</v>
@@ -9627,7 +9622,7 @@
         <v>59</v>
       </c>
       <c r="AK67" t="s" s="2">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="AL67" t="s" s="2">
         <v>37</v>
@@ -9636,7 +9631,7 @@
         <v>67</v>
       </c>
       <c r="AN67" t="s" s="2">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="AO67" t="s" s="2">
         <v>37</v>
@@ -9644,10 +9639,10 @@
     </row>
     <row r="68" hidden="true">
       <c r="A68" t="s" s="2">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B68" t="s" s="2">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="C68" s="2"/>
       <c r="D68" t="s" s="2">
@@ -9670,13 +9665,13 @@
         <v>37</v>
       </c>
       <c r="K68" t="s" s="2">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="L68" t="s" s="2">
+        <v>440</v>
+      </c>
+      <c r="M68" t="s" s="2">
         <v>441</v>
-      </c>
-      <c r="M68" t="s" s="2">
-        <v>442</v>
       </c>
       <c r="N68" s="2"/>
       <c r="O68" s="2"/>
@@ -9727,7 +9722,7 @@
         <v>37</v>
       </c>
       <c r="AF68" t="s" s="2">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="AG68" t="s" s="2">
         <v>35</v>
@@ -9742,7 +9737,7 @@
         <v>59</v>
       </c>
       <c r="AK68" t="s" s="2">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="AL68" t="s" s="2">
         <v>37</v>
@@ -9759,10 +9754,10 @@
     </row>
     <row r="69" hidden="true">
       <c r="A69" t="s" s="2">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B69" t="s" s="2">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="C69" s="2"/>
       <c r="D69" t="s" s="2">
@@ -9874,10 +9869,10 @@
     </row>
     <row r="70" hidden="true">
       <c r="A70" t="s" s="2">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B70" t="s" s="2">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="C70" s="2"/>
       <c r="D70" t="s" s="2">
@@ -9991,14 +9986,14 @@
     </row>
     <row r="71" hidden="true">
       <c r="A71" t="s" s="2">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B71" t="s" s="2">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C71" s="2"/>
       <c r="D71" t="s" s="2">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="E71" s="2"/>
       <c r="F71" t="s" s="2">
@@ -10020,10 +10015,10 @@
         <v>94</v>
       </c>
       <c r="L71" t="s" s="2">
+        <v>421</v>
+      </c>
+      <c r="M71" t="s" s="2">
         <v>422</v>
-      </c>
-      <c r="M71" t="s" s="2">
-        <v>423</v>
       </c>
       <c r="N71" t="s" s="2">
         <v>97</v>
@@ -10078,7 +10073,7 @@
         <v>37</v>
       </c>
       <c r="AF71" t="s" s="2">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="AG71" t="s" s="2">
         <v>35</v>
@@ -10110,10 +10105,10 @@
     </row>
     <row r="72" hidden="true">
       <c r="A72" t="s" s="2">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B72" t="s" s="2">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="C72" s="2"/>
       <c r="D72" t="s" s="2">
@@ -10139,10 +10134,10 @@
         <v>155</v>
       </c>
       <c r="L72" t="s" s="2">
+        <v>447</v>
+      </c>
+      <c r="M72" t="s" s="2">
         <v>448</v>
-      </c>
-      <c r="M72" t="s" s="2">
-        <v>449</v>
       </c>
       <c r="N72" t="s" s="2">
         <v>241</v>
@@ -10195,7 +10190,7 @@
         <v>37</v>
       </c>
       <c r="AF72" t="s" s="2">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="AG72" t="s" s="2">
         <v>35</v>
@@ -10210,7 +10205,7 @@
         <v>59</v>
       </c>
       <c r="AK72" t="s" s="2">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="AL72" t="s" s="2">
         <v>37</v>
@@ -10227,10 +10222,10 @@
     </row>
     <row r="73" hidden="true">
       <c r="A73" t="s" s="2">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B73" t="s" s="2">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="C73" s="2"/>
       <c r="D73" t="s" s="2">
@@ -10256,10 +10251,10 @@
         <v>177</v>
       </c>
       <c r="L73" t="s" s="2">
+        <v>451</v>
+      </c>
+      <c r="M73" t="s" s="2">
         <v>452</v>
-      </c>
-      <c r="M73" t="s" s="2">
-        <v>453</v>
       </c>
       <c r="N73" t="s" s="2">
         <v>271</v>
@@ -10291,11 +10286,11 @@
         <v>73</v>
       </c>
       <c r="Y73" t="s" s="2">
+        <v>453</v>
+      </c>
+      <c r="Z73" t="s" s="2">
         <v>454</v>
       </c>
-      <c r="Z73" t="s" s="2">
-        <v>455</v>
-      </c>
       <c r="AA73" t="s" s="2">
         <v>37</v>
       </c>
@@ -10312,7 +10307,7 @@
         <v>37</v>
       </c>
       <c r="AF73" t="s" s="2">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="AG73" t="s" s="2">
         <v>35</v>
@@ -10327,7 +10322,7 @@
         <v>59</v>
       </c>
       <c r="AK73" t="s" s="2">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="AL73" t="s" s="2">
         <v>275</v>

</xml_diff>

<commit_message>
informations manquantes sur les contacts (#67)
* MaJ mapping contact

* ajout extensions pour le contact

ajout des extensons :
ECLAIREContactAddress
ECLAIREContactAffiliation
ECLAIREContactName

* typo

* Correction typo mapping

* Maj mapping nom contact

---------

Co-authored-by: sly-kereval <125375447+sly-kereval@users.noreply.github.com> 0ee375f61403042653f42344f224f21ab8fb705a
</commit_message>
<xml_diff>
--- a/ig/main/StructureDefinition-eclaire-researchstudy.xlsx
+++ b/ig/main/StructureDefinition-eclaire-researchstudy.xlsx
@@ -10,13 +10,13 @@
     <sheet name="Elements" r:id="rId4" sheetId="2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="true">Elements!$A$1:$AO$73</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="true">Elements!$A$1:$AO$76</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2736" uniqueCount="457">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2847" uniqueCount="472">
   <si>
     <t>Property</t>
   </si>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-09-22T15:13:42+00:00</t>
+    <t>2023-10-04T13:47:44+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -1005,10 +1005,58 @@
 </t>
   </si>
   <si>
-    <t>type de contact : Public ou Scientific</t>
+    <t>Type de contact : Public ou Scientific</t>
   </si>
   <si>
     <t>Extension créée dans le cadre du projet ECLAIRE qui indique le type de Contact : Public ou Scientific</t>
+  </si>
+  <si>
+    <t>ResearchStudy.contact.extension:eclaire-contact-address</t>
+  </si>
+  <si>
+    <t>eclaire-contact-address</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extension {https://interop.esante.gouv.fr/ig/fhir/eclaire/StructureDefinition/eclaire-contact-address}
+</t>
+  </si>
+  <si>
+    <t>Adresse du contact</t>
+  </si>
+  <si>
+    <t>Extension créée dans le cadre du projet ECLAIRE pour indiquer l'adresse du contact</t>
+  </si>
+  <si>
+    <t>ResearchStudy.contact.extension:eclaire-contact-affiliation</t>
+  </si>
+  <si>
+    <t>eclaire-contact-affiliation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extension {https://interop.esante.gouv.fr/ig/fhir/eclaire/StructureDefinition/eclaire-contact-affiliation}
+</t>
+  </si>
+  <si>
+    <t>Affiliation du contact</t>
+  </si>
+  <si>
+    <t>Extension créée dans le cadre du projet ECLAIRE pour indiquer l'affiliation du contact</t>
+  </si>
+  <si>
+    <t>ResearchStudy.contact.extension:eclaire-contact-name</t>
+  </si>
+  <si>
+    <t>eclaire-contact-name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extension {https://interop.esante.gouv.fr/ig/fhir/eclaire/StructureDefinition/eclaire-contact-name}
+</t>
+  </si>
+  <si>
+    <t>Nom du contact</t>
+  </si>
+  <si>
+    <t>Extension créée dans le cadre du projet ECLAIRE pour indiquer le nom de contact</t>
   </si>
   <si>
     <t>ResearchStudy.contact.name</t>
@@ -1748,7 +1796,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AO73"/>
+  <dimension ref="A1:AO76"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -1757,7 +1805,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="50.921875" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="55.40234375" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="41.0234375" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="25.26171875" customWidth="true" bestFit="true" hidden="true"/>
     <col min="4" max="4" width="39.9140625" customWidth="true" bestFit="true" hidden="true"/>
@@ -7310,9 +7358,11 @@
         <v>318</v>
       </c>
       <c r="B48" t="s" s="2">
-        <v>318</v>
-      </c>
-      <c r="C48" s="2"/>
+        <v>312</v>
+      </c>
+      <c r="C48" t="s" s="2">
+        <v>319</v>
+      </c>
       <c r="D48" t="s" s="2">
         <v>37</v>
       </c>
@@ -7324,26 +7374,24 @@
         <v>47</v>
       </c>
       <c r="H48" t="s" s="2">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="I48" t="s" s="2">
         <v>37</v>
       </c>
       <c r="J48" t="s" s="2">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="K48" t="s" s="2">
-        <v>156</v>
+        <v>320</v>
       </c>
       <c r="L48" t="s" s="2">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="M48" t="s" s="2">
-        <v>320</v>
-      </c>
-      <c r="N48" t="s" s="2">
-        <v>321</v>
-      </c>
+        <v>322</v>
+      </c>
+      <c r="N48" s="2"/>
       <c r="O48" s="2"/>
       <c r="P48" t="s" s="2">
         <v>37</v>
@@ -7392,19 +7440,19 @@
         <v>37</v>
       </c>
       <c r="AF48" t="s" s="2">
-        <v>322</v>
+        <v>163</v>
       </c>
       <c r="AG48" t="s" s="2">
         <v>35</v>
       </c>
       <c r="AH48" t="s" s="2">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="AI48" t="s" s="2">
         <v>59</v>
       </c>
       <c r="AJ48" t="s" s="2">
-        <v>60</v>
+        <v>103</v>
       </c>
       <c r="AK48" t="s" s="2">
         <v>37</v>
@@ -7413,7 +7461,7 @@
         <v>37</v>
       </c>
       <c r="AM48" t="s" s="2">
-        <v>68</v>
+        <v>37</v>
       </c>
       <c r="AN48" t="s" s="2">
         <v>37</v>
@@ -7427,9 +7475,11 @@
         <v>323</v>
       </c>
       <c r="B49" t="s" s="2">
-        <v>323</v>
-      </c>
-      <c r="C49" s="2"/>
+        <v>312</v>
+      </c>
+      <c r="C49" t="s" s="2">
+        <v>324</v>
+      </c>
       <c r="D49" t="s" s="2">
         <v>37</v>
       </c>
@@ -7438,25 +7488,25 @@
         <v>35</v>
       </c>
       <c r="G49" t="s" s="2">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="H49" t="s" s="2">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="I49" t="s" s="2">
         <v>37</v>
       </c>
       <c r="J49" t="s" s="2">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="K49" t="s" s="2">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="L49" t="s" s="2">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="M49" t="s" s="2">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="N49" s="2"/>
       <c r="O49" s="2"/>
@@ -7507,7 +7557,7 @@
         <v>37</v>
       </c>
       <c r="AF49" t="s" s="2">
-        <v>327</v>
+        <v>163</v>
       </c>
       <c r="AG49" t="s" s="2">
         <v>35</v>
@@ -7519,16 +7569,16 @@
         <v>59</v>
       </c>
       <c r="AJ49" t="s" s="2">
-        <v>328</v>
+        <v>103</v>
       </c>
       <c r="AK49" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AL49" t="s" s="2">
-        <v>329</v>
+        <v>37</v>
       </c>
       <c r="AM49" t="s" s="2">
-        <v>330</v>
+        <v>37</v>
       </c>
       <c r="AN49" t="s" s="2">
         <v>37</v>
@@ -7539,12 +7589,14 @@
     </row>
     <row r="50" hidden="true">
       <c r="A50" t="s" s="2">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="B50" t="s" s="2">
-        <v>331</v>
-      </c>
-      <c r="C50" s="2"/>
+        <v>312</v>
+      </c>
+      <c r="C50" t="s" s="2">
+        <v>329</v>
+      </c>
       <c r="D50" t="s" s="2">
         <v>37</v>
       </c>
@@ -7553,7 +7605,7 @@
         <v>35</v>
       </c>
       <c r="G50" t="s" s="2">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="H50" t="s" s="2">
         <v>37</v>
@@ -7565,17 +7617,15 @@
         <v>37</v>
       </c>
       <c r="K50" t="s" s="2">
+        <v>330</v>
+      </c>
+      <c r="L50" t="s" s="2">
+        <v>331</v>
+      </c>
+      <c r="M50" t="s" s="2">
         <v>332</v>
       </c>
-      <c r="L50" t="s" s="2">
-        <v>333</v>
-      </c>
-      <c r="M50" t="s" s="2">
-        <v>334</v>
-      </c>
-      <c r="N50" t="s" s="2">
-        <v>335</v>
-      </c>
+      <c r="N50" s="2"/>
       <c r="O50" s="2"/>
       <c r="P50" t="s" s="2">
         <v>37</v>
@@ -7624,7 +7674,7 @@
         <v>37</v>
       </c>
       <c r="AF50" t="s" s="2">
-        <v>331</v>
+        <v>163</v>
       </c>
       <c r="AG50" t="s" s="2">
         <v>35</v>
@@ -7636,19 +7686,19 @@
         <v>59</v>
       </c>
       <c r="AJ50" t="s" s="2">
-        <v>60</v>
+        <v>103</v>
       </c>
       <c r="AK50" t="s" s="2">
-        <v>336</v>
+        <v>37</v>
       </c>
       <c r="AL50" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AM50" t="s" s="2">
-        <v>68</v>
+        <v>37</v>
       </c>
       <c r="AN50" t="s" s="2">
-        <v>337</v>
+        <v>37</v>
       </c>
       <c r="AO50" t="s" s="2">
         <v>37</v>
@@ -7656,10 +7706,10 @@
     </row>
     <row r="51" hidden="true">
       <c r="A51" t="s" s="2">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="B51" t="s" s="2">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="C51" s="2"/>
       <c r="D51" t="s" s="2">
@@ -7670,7 +7720,7 @@
         <v>35</v>
       </c>
       <c r="G51" t="s" s="2">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="H51" t="s" s="2">
         <v>37</v>
@@ -7682,16 +7732,16 @@
         <v>48</v>
       </c>
       <c r="K51" t="s" s="2">
-        <v>178</v>
+        <v>156</v>
       </c>
       <c r="L51" t="s" s="2">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="M51" t="s" s="2">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="N51" t="s" s="2">
-        <v>272</v>
+        <v>336</v>
       </c>
       <c r="O51" s="2"/>
       <c r="P51" t="s" s="2">
@@ -7717,10 +7767,10 @@
         <v>37</v>
       </c>
       <c r="X51" t="s" s="2">
-        <v>287</v>
+        <v>37</v>
       </c>
       <c r="Y51" t="s" s="2">
-        <v>341</v>
+        <v>37</v>
       </c>
       <c r="Z51" t="s" s="2">
         <v>37</v>
@@ -7741,13 +7791,13 @@
         <v>37</v>
       </c>
       <c r="AF51" t="s" s="2">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="AG51" t="s" s="2">
         <v>35</v>
       </c>
       <c r="AH51" t="s" s="2">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="AI51" t="s" s="2">
         <v>59</v>
@@ -7756,16 +7806,16 @@
         <v>60</v>
       </c>
       <c r="AK51" t="s" s="2">
-        <v>342</v>
+        <v>37</v>
       </c>
       <c r="AL51" t="s" s="2">
-        <v>276</v>
+        <v>37</v>
       </c>
       <c r="AM51" t="s" s="2">
-        <v>277</v>
+        <v>68</v>
       </c>
       <c r="AN51" t="s" s="2">
-        <v>343</v>
+        <v>37</v>
       </c>
       <c r="AO51" t="s" s="2">
         <v>37</v>
@@ -7773,10 +7823,10 @@
     </row>
     <row r="52" hidden="true">
       <c r="A52" t="s" s="2">
-        <v>344</v>
+        <v>338</v>
       </c>
       <c r="B52" t="s" s="2">
-        <v>344</v>
+        <v>338</v>
       </c>
       <c r="C52" s="2"/>
       <c r="D52" t="s" s="2">
@@ -7790,7 +7840,7 @@
         <v>36</v>
       </c>
       <c r="H52" t="s" s="2">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="I52" t="s" s="2">
         <v>37</v>
@@ -7799,17 +7849,15 @@
         <v>48</v>
       </c>
       <c r="K52" t="s" s="2">
-        <v>178</v>
+        <v>339</v>
       </c>
       <c r="L52" t="s" s="2">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="M52" t="s" s="2">
-        <v>346</v>
-      </c>
-      <c r="N52" t="s" s="2">
-        <v>272</v>
-      </c>
+        <v>341</v>
+      </c>
+      <c r="N52" s="2"/>
       <c r="O52" s="2"/>
       <c r="P52" t="s" s="2">
         <v>37</v>
@@ -7834,13 +7882,13 @@
         <v>37</v>
       </c>
       <c r="X52" t="s" s="2">
-        <v>183</v>
+        <v>37</v>
       </c>
       <c r="Y52" t="s" s="2">
-        <v>347</v>
+        <v>37</v>
       </c>
       <c r="Z52" t="s" s="2">
-        <v>348</v>
+        <v>37</v>
       </c>
       <c r="AA52" t="s" s="2">
         <v>37</v>
@@ -7858,7 +7906,7 @@
         <v>37</v>
       </c>
       <c r="AF52" t="s" s="2">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="AG52" t="s" s="2">
         <v>35</v>
@@ -7870,16 +7918,16 @@
         <v>59</v>
       </c>
       <c r="AJ52" t="s" s="2">
-        <v>60</v>
+        <v>343</v>
       </c>
       <c r="AK52" t="s" s="2">
-        <v>349</v>
+        <v>37</v>
       </c>
       <c r="AL52" t="s" s="2">
-        <v>276</v>
+        <v>344</v>
       </c>
       <c r="AM52" t="s" s="2">
-        <v>277</v>
+        <v>345</v>
       </c>
       <c r="AN52" t="s" s="2">
         <v>37</v>
@@ -7890,10 +7938,10 @@
     </row>
     <row r="53" hidden="true">
       <c r="A53" t="s" s="2">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="B53" t="s" s="2">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="C53" s="2"/>
       <c r="D53" t="s" s="2">
@@ -7904,10 +7952,10 @@
         <v>35</v>
       </c>
       <c r="G53" t="s" s="2">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="H53" t="s" s="2">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="I53" t="s" s="2">
         <v>37</v>
@@ -7916,16 +7964,16 @@
         <v>37</v>
       </c>
       <c r="K53" t="s" s="2">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="L53" t="s" s="2">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="M53" t="s" s="2">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="N53" t="s" s="2">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="O53" s="2"/>
       <c r="P53" t="s" s="2">
@@ -7975,13 +8023,13 @@
         <v>37</v>
       </c>
       <c r="AF53" t="s" s="2">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="AG53" t="s" s="2">
         <v>35</v>
       </c>
       <c r="AH53" t="s" s="2">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="AI53" t="s" s="2">
         <v>59</v>
@@ -7990,7 +8038,7 @@
         <v>60</v>
       </c>
       <c r="AK53" t="s" s="2">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="AL53" t="s" s="2">
         <v>37</v>
@@ -7999,7 +8047,7 @@
         <v>68</v>
       </c>
       <c r="AN53" t="s" s="2">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="AO53" t="s" s="2">
         <v>37</v>
@@ -8007,14 +8055,14 @@
     </row>
     <row r="54" hidden="true">
       <c r="A54" t="s" s="2">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="B54" t="s" s="2">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="C54" s="2"/>
       <c r="D54" t="s" s="2">
-        <v>358</v>
+        <v>37</v>
       </c>
       <c r="E54" s="2"/>
       <c r="F54" t="s" s="2">
@@ -8024,7 +8072,7 @@
         <v>36</v>
       </c>
       <c r="H54" t="s" s="2">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="I54" t="s" s="2">
         <v>37</v>
@@ -8033,16 +8081,16 @@
         <v>48</v>
       </c>
       <c r="K54" t="s" s="2">
-        <v>359</v>
+        <v>178</v>
       </c>
       <c r="L54" t="s" s="2">
-        <v>360</v>
+        <v>354</v>
       </c>
       <c r="M54" t="s" s="2">
-        <v>361</v>
+        <v>355</v>
       </c>
       <c r="N54" t="s" s="2">
-        <v>362</v>
+        <v>272</v>
       </c>
       <c r="O54" s="2"/>
       <c r="P54" t="s" s="2">
@@ -8068,10 +8116,10 @@
         <v>37</v>
       </c>
       <c r="X54" t="s" s="2">
-        <v>37</v>
+        <v>287</v>
       </c>
       <c r="Y54" t="s" s="2">
-        <v>37</v>
+        <v>356</v>
       </c>
       <c r="Z54" t="s" s="2">
         <v>37</v>
@@ -8092,7 +8140,7 @@
         <v>37</v>
       </c>
       <c r="AF54" t="s" s="2">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="AG54" t="s" s="2">
         <v>35</v>
@@ -8104,44 +8152,44 @@
         <v>59</v>
       </c>
       <c r="AJ54" t="s" s="2">
-        <v>224</v>
+        <v>60</v>
       </c>
       <c r="AK54" t="s" s="2">
-        <v>363</v>
+        <v>357</v>
       </c>
       <c r="AL54" t="s" s="2">
-        <v>37</v>
+        <v>276</v>
       </c>
       <c r="AM54" t="s" s="2">
-        <v>364</v>
+        <v>277</v>
       </c>
       <c r="AN54" t="s" s="2">
-        <v>365</v>
+        <v>358</v>
       </c>
       <c r="AO54" t="s" s="2">
-        <v>366</v>
+        <v>37</v>
       </c>
     </row>
     <row r="55" hidden="true">
       <c r="A55" t="s" s="2">
-        <v>367</v>
+        <v>359</v>
       </c>
       <c r="B55" t="s" s="2">
-        <v>367</v>
+        <v>359</v>
       </c>
       <c r="C55" s="2"/>
       <c r="D55" t="s" s="2">
-        <v>368</v>
+        <v>37</v>
       </c>
       <c r="E55" s="2"/>
       <c r="F55" t="s" s="2">
         <v>35</v>
       </c>
       <c r="G55" t="s" s="2">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="H55" t="s" s="2">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="I55" t="s" s="2">
         <v>37</v>
@@ -8150,16 +8198,16 @@
         <v>48</v>
       </c>
       <c r="K55" t="s" s="2">
-        <v>209</v>
+        <v>178</v>
       </c>
       <c r="L55" t="s" s="2">
-        <v>369</v>
+        <v>360</v>
       </c>
       <c r="M55" t="s" s="2">
-        <v>370</v>
+        <v>361</v>
       </c>
       <c r="N55" t="s" s="2">
-        <v>212</v>
+        <v>272</v>
       </c>
       <c r="O55" s="2"/>
       <c r="P55" t="s" s="2">
@@ -8185,13 +8233,13 @@
         <v>37</v>
       </c>
       <c r="X55" t="s" s="2">
-        <v>37</v>
+        <v>183</v>
       </c>
       <c r="Y55" t="s" s="2">
-        <v>37</v>
+        <v>362</v>
       </c>
       <c r="Z55" t="s" s="2">
-        <v>37</v>
+        <v>363</v>
       </c>
       <c r="AA55" t="s" s="2">
         <v>37</v>
@@ -8209,42 +8257,42 @@
         <v>37</v>
       </c>
       <c r="AF55" t="s" s="2">
-        <v>367</v>
+        <v>359</v>
       </c>
       <c r="AG55" t="s" s="2">
         <v>35</v>
       </c>
       <c r="AH55" t="s" s="2">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="AI55" t="s" s="2">
         <v>59</v>
       </c>
       <c r="AJ55" t="s" s="2">
-        <v>214</v>
+        <v>60</v>
       </c>
       <c r="AK55" t="s" s="2">
-        <v>371</v>
+        <v>364</v>
       </c>
       <c r="AL55" t="s" s="2">
-        <v>372</v>
+        <v>276</v>
       </c>
       <c r="AM55" t="s" s="2">
-        <v>373</v>
+        <v>277</v>
       </c>
       <c r="AN55" t="s" s="2">
-        <v>374</v>
+        <v>37</v>
       </c>
       <c r="AO55" t="s" s="2">
-        <v>375</v>
+        <v>37</v>
       </c>
     </row>
     <row r="56" hidden="true">
       <c r="A56" t="s" s="2">
-        <v>376</v>
+        <v>365</v>
       </c>
       <c r="B56" t="s" s="2">
-        <v>376</v>
+        <v>365</v>
       </c>
       <c r="C56" s="2"/>
       <c r="D56" t="s" s="2">
@@ -8264,19 +8312,19 @@
         <v>37</v>
       </c>
       <c r="J56" t="s" s="2">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="K56" t="s" s="2">
-        <v>219</v>
+        <v>366</v>
       </c>
       <c r="L56" t="s" s="2">
-        <v>377</v>
+        <v>367</v>
       </c>
       <c r="M56" t="s" s="2">
-        <v>378</v>
+        <v>368</v>
       </c>
       <c r="N56" t="s" s="2">
-        <v>249</v>
+        <v>369</v>
       </c>
       <c r="O56" s="2"/>
       <c r="P56" t="s" s="2">
@@ -8326,7 +8374,7 @@
         <v>37</v>
       </c>
       <c r="AF56" t="s" s="2">
-        <v>376</v>
+        <v>365</v>
       </c>
       <c r="AG56" t="s" s="2">
         <v>35</v>
@@ -8338,44 +8386,44 @@
         <v>59</v>
       </c>
       <c r="AJ56" t="s" s="2">
-        <v>224</v>
+        <v>60</v>
       </c>
       <c r="AK56" t="s" s="2">
-        <v>379</v>
+        <v>370</v>
       </c>
       <c r="AL56" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AM56" t="s" s="2">
-        <v>380</v>
+        <v>68</v>
       </c>
       <c r="AN56" t="s" s="2">
-        <v>381</v>
+        <v>371</v>
       </c>
       <c r="AO56" t="s" s="2">
-        <v>382</v>
+        <v>37</v>
       </c>
     </row>
     <row r="57" hidden="true">
       <c r="A57" t="s" s="2">
-        <v>383</v>
+        <v>372</v>
       </c>
       <c r="B57" t="s" s="2">
-        <v>383</v>
+        <v>372</v>
       </c>
       <c r="C57" s="2"/>
       <c r="D57" t="s" s="2">
-        <v>37</v>
+        <v>373</v>
       </c>
       <c r="E57" s="2"/>
       <c r="F57" t="s" s="2">
         <v>35</v>
       </c>
       <c r="G57" t="s" s="2">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="H57" t="s" s="2">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="I57" t="s" s="2">
         <v>37</v>
@@ -8384,16 +8432,16 @@
         <v>48</v>
       </c>
       <c r="K57" t="s" s="2">
-        <v>384</v>
+        <v>374</v>
       </c>
       <c r="L57" t="s" s="2">
-        <v>385</v>
+        <v>375</v>
       </c>
       <c r="M57" t="s" s="2">
-        <v>386</v>
+        <v>376</v>
       </c>
       <c r="N57" t="s" s="2">
-        <v>249</v>
+        <v>377</v>
       </c>
       <c r="O57" s="2"/>
       <c r="P57" t="s" s="2">
@@ -8443,13 +8491,13 @@
         <v>37</v>
       </c>
       <c r="AF57" t="s" s="2">
-        <v>383</v>
+        <v>372</v>
       </c>
       <c r="AG57" t="s" s="2">
         <v>35</v>
       </c>
       <c r="AH57" t="s" s="2">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="AI57" t="s" s="2">
         <v>59</v>
@@ -8458,41 +8506,41 @@
         <v>224</v>
       </c>
       <c r="AK57" t="s" s="2">
-        <v>387</v>
+        <v>378</v>
       </c>
       <c r="AL57" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AM57" t="s" s="2">
-        <v>388</v>
+        <v>379</v>
       </c>
       <c r="AN57" t="s" s="2">
-        <v>389</v>
+        <v>380</v>
       </c>
       <c r="AO57" t="s" s="2">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="58" hidden="true">
       <c r="A58" t="s" s="2">
-        <v>390</v>
+        <v>382</v>
       </c>
       <c r="B58" t="s" s="2">
-        <v>390</v>
+        <v>382</v>
       </c>
       <c r="C58" s="2"/>
       <c r="D58" t="s" s="2">
-        <v>37</v>
+        <v>383</v>
       </c>
       <c r="E58" s="2"/>
       <c r="F58" t="s" s="2">
         <v>35</v>
       </c>
       <c r="G58" t="s" s="2">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="H58" t="s" s="2">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="I58" t="s" s="2">
         <v>37</v>
@@ -8501,16 +8549,16 @@
         <v>48</v>
       </c>
       <c r="K58" t="s" s="2">
-        <v>391</v>
+        <v>209</v>
       </c>
       <c r="L58" t="s" s="2">
-        <v>392</v>
+        <v>384</v>
       </c>
       <c r="M58" t="s" s="2">
-        <v>393</v>
+        <v>385</v>
       </c>
       <c r="N58" t="s" s="2">
-        <v>249</v>
+        <v>212</v>
       </c>
       <c r="O58" s="2"/>
       <c r="P58" t="s" s="2">
@@ -8560,42 +8608,42 @@
         <v>37</v>
       </c>
       <c r="AF58" t="s" s="2">
-        <v>390</v>
+        <v>382</v>
       </c>
       <c r="AG58" t="s" s="2">
         <v>35</v>
       </c>
       <c r="AH58" t="s" s="2">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="AI58" t="s" s="2">
         <v>59</v>
       </c>
       <c r="AJ58" t="s" s="2">
-        <v>224</v>
+        <v>214</v>
       </c>
       <c r="AK58" t="s" s="2">
-        <v>394</v>
+        <v>386</v>
       </c>
       <c r="AL58" t="s" s="2">
-        <v>37</v>
+        <v>387</v>
       </c>
       <c r="AM58" t="s" s="2">
         <v>388</v>
       </c>
       <c r="AN58" t="s" s="2">
-        <v>395</v>
+        <v>389</v>
       </c>
       <c r="AO58" t="s" s="2">
-        <v>396</v>
+        <v>390</v>
       </c>
     </row>
     <row r="59" hidden="true">
       <c r="A59" t="s" s="2">
-        <v>397</v>
+        <v>391</v>
       </c>
       <c r="B59" t="s" s="2">
-        <v>397</v>
+        <v>391</v>
       </c>
       <c r="C59" s="2"/>
       <c r="D59" t="s" s="2">
@@ -8609,7 +8657,7 @@
         <v>47</v>
       </c>
       <c r="H59" t="s" s="2">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="I59" t="s" s="2">
         <v>37</v>
@@ -8618,16 +8666,16 @@
         <v>48</v>
       </c>
       <c r="K59" t="s" s="2">
-        <v>178</v>
+        <v>219</v>
       </c>
       <c r="L59" t="s" s="2">
-        <v>398</v>
+        <v>392</v>
       </c>
       <c r="M59" t="s" s="2">
-        <v>399</v>
+        <v>393</v>
       </c>
       <c r="N59" t="s" s="2">
-        <v>272</v>
+        <v>249</v>
       </c>
       <c r="O59" s="2"/>
       <c r="P59" t="s" s="2">
@@ -8653,13 +8701,13 @@
         <v>37</v>
       </c>
       <c r="X59" t="s" s="2">
-        <v>287</v>
+        <v>37</v>
       </c>
       <c r="Y59" t="s" s="2">
-        <v>400</v>
+        <v>37</v>
       </c>
       <c r="Z59" t="s" s="2">
-        <v>401</v>
+        <v>37</v>
       </c>
       <c r="AA59" t="s" s="2">
         <v>37</v>
@@ -8677,7 +8725,7 @@
         <v>37</v>
       </c>
       <c r="AF59" t="s" s="2">
-        <v>397</v>
+        <v>391</v>
       </c>
       <c r="AG59" t="s" s="2">
         <v>35</v>
@@ -8689,30 +8737,30 @@
         <v>59</v>
       </c>
       <c r="AJ59" t="s" s="2">
-        <v>60</v>
+        <v>224</v>
       </c>
       <c r="AK59" t="s" s="2">
-        <v>402</v>
+        <v>394</v>
       </c>
       <c r="AL59" t="s" s="2">
-        <v>276</v>
+        <v>37</v>
       </c>
       <c r="AM59" t="s" s="2">
-        <v>277</v>
+        <v>395</v>
       </c>
       <c r="AN59" t="s" s="2">
-        <v>403</v>
+        <v>396</v>
       </c>
       <c r="AO59" t="s" s="2">
-        <v>404</v>
+        <v>397</v>
       </c>
     </row>
     <row r="60" hidden="true">
       <c r="A60" t="s" s="2">
-        <v>405</v>
+        <v>398</v>
       </c>
       <c r="B60" t="s" s="2">
-        <v>405</v>
+        <v>398</v>
       </c>
       <c r="C60" s="2"/>
       <c r="D60" t="s" s="2">
@@ -8723,7 +8771,7 @@
         <v>35</v>
       </c>
       <c r="G60" t="s" s="2">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="H60" t="s" s="2">
         <v>37</v>
@@ -8732,19 +8780,19 @@
         <v>37</v>
       </c>
       <c r="J60" t="s" s="2">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="K60" t="s" s="2">
-        <v>406</v>
+        <v>399</v>
       </c>
       <c r="L60" t="s" s="2">
-        <v>407</v>
+        <v>400</v>
       </c>
       <c r="M60" t="s" s="2">
-        <v>408</v>
+        <v>401</v>
       </c>
       <c r="N60" t="s" s="2">
-        <v>409</v>
+        <v>249</v>
       </c>
       <c r="O60" s="2"/>
       <c r="P60" t="s" s="2">
@@ -8794,42 +8842,42 @@
         <v>37</v>
       </c>
       <c r="AF60" t="s" s="2">
-        <v>405</v>
+        <v>398</v>
       </c>
       <c r="AG60" t="s" s="2">
         <v>35</v>
       </c>
       <c r="AH60" t="s" s="2">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="AI60" t="s" s="2">
         <v>59</v>
       </c>
       <c r="AJ60" t="s" s="2">
-        <v>60</v>
+        <v>224</v>
       </c>
       <c r="AK60" t="s" s="2">
-        <v>410</v>
+        <v>402</v>
       </c>
       <c r="AL60" t="s" s="2">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="AM60" t="s" s="2">
-        <v>411</v>
+        <v>403</v>
       </c>
       <c r="AN60" t="s" s="2">
-        <v>37</v>
+        <v>404</v>
       </c>
       <c r="AO60" t="s" s="2">
-        <v>37</v>
+        <v>397</v>
       </c>
     </row>
     <row r="61" hidden="true">
       <c r="A61" t="s" s="2">
-        <v>412</v>
+        <v>405</v>
       </c>
       <c r="B61" t="s" s="2">
-        <v>412</v>
+        <v>405</v>
       </c>
       <c r="C61" s="2"/>
       <c r="D61" t="s" s="2">
@@ -8843,24 +8891,26 @@
         <v>36</v>
       </c>
       <c r="H61" t="s" s="2">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="I61" t="s" s="2">
         <v>37</v>
       </c>
       <c r="J61" t="s" s="2">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="K61" t="s" s="2">
-        <v>413</v>
+        <v>406</v>
       </c>
       <c r="L61" t="s" s="2">
-        <v>414</v>
+        <v>407</v>
       </c>
       <c r="M61" t="s" s="2">
-        <v>415</v>
-      </c>
-      <c r="N61" s="2"/>
+        <v>408</v>
+      </c>
+      <c r="N61" t="s" s="2">
+        <v>249</v>
+      </c>
       <c r="O61" s="2"/>
       <c r="P61" t="s" s="2">
         <v>37</v>
@@ -8909,7 +8959,7 @@
         <v>37</v>
       </c>
       <c r="AF61" t="s" s="2">
-        <v>412</v>
+        <v>405</v>
       </c>
       <c r="AG61" t="s" s="2">
         <v>35</v>
@@ -8921,30 +8971,30 @@
         <v>59</v>
       </c>
       <c r="AJ61" t="s" s="2">
-        <v>60</v>
+        <v>224</v>
       </c>
       <c r="AK61" t="s" s="2">
-        <v>416</v>
+        <v>409</v>
       </c>
       <c r="AL61" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AM61" t="s" s="2">
-        <v>68</v>
+        <v>403</v>
       </c>
       <c r="AN61" t="s" s="2">
-        <v>417</v>
+        <v>410</v>
       </c>
       <c r="AO61" t="s" s="2">
-        <v>37</v>
+        <v>411</v>
       </c>
     </row>
     <row r="62" hidden="true">
       <c r="A62" t="s" s="2">
-        <v>418</v>
+        <v>412</v>
       </c>
       <c r="B62" t="s" s="2">
-        <v>418</v>
+        <v>412</v>
       </c>
       <c r="C62" s="2"/>
       <c r="D62" t="s" s="2">
@@ -8964,18 +9014,20 @@
         <v>37</v>
       </c>
       <c r="J62" t="s" s="2">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="K62" t="s" s="2">
-        <v>156</v>
+        <v>178</v>
       </c>
       <c r="L62" t="s" s="2">
-        <v>157</v>
+        <v>413</v>
       </c>
       <c r="M62" t="s" s="2">
-        <v>158</v>
-      </c>
-      <c r="N62" s="2"/>
+        <v>414</v>
+      </c>
+      <c r="N62" t="s" s="2">
+        <v>272</v>
+      </c>
       <c r="O62" s="2"/>
       <c r="P62" t="s" s="2">
         <v>37</v>
@@ -9000,13 +9052,13 @@
         <v>37</v>
       </c>
       <c r="X62" t="s" s="2">
-        <v>37</v>
+        <v>287</v>
       </c>
       <c r="Y62" t="s" s="2">
-        <v>37</v>
+        <v>415</v>
       </c>
       <c r="Z62" t="s" s="2">
-        <v>37</v>
+        <v>416</v>
       </c>
       <c r="AA62" t="s" s="2">
         <v>37</v>
@@ -9024,7 +9076,7 @@
         <v>37</v>
       </c>
       <c r="AF62" t="s" s="2">
-        <v>159</v>
+        <v>412</v>
       </c>
       <c r="AG62" t="s" s="2">
         <v>35</v>
@@ -9033,37 +9085,37 @@
         <v>47</v>
       </c>
       <c r="AI62" t="s" s="2">
-        <v>37</v>
+        <v>59</v>
       </c>
       <c r="AJ62" t="s" s="2">
-        <v>37</v>
+        <v>60</v>
       </c>
       <c r="AK62" t="s" s="2">
-        <v>37</v>
+        <v>417</v>
       </c>
       <c r="AL62" t="s" s="2">
-        <v>37</v>
+        <v>276</v>
       </c>
       <c r="AM62" t="s" s="2">
-        <v>68</v>
+        <v>277</v>
       </c>
       <c r="AN62" t="s" s="2">
-        <v>37</v>
+        <v>418</v>
       </c>
       <c r="AO62" t="s" s="2">
-        <v>37</v>
+        <v>419</v>
       </c>
     </row>
     <row r="63" hidden="true">
       <c r="A63" t="s" s="2">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="B63" t="s" s="2">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="C63" s="2"/>
       <c r="D63" t="s" s="2">
-        <v>94</v>
+        <v>37</v>
       </c>
       <c r="E63" s="2"/>
       <c r="F63" t="s" s="2">
@@ -9082,16 +9134,16 @@
         <v>37</v>
       </c>
       <c r="K63" t="s" s="2">
-        <v>95</v>
+        <v>421</v>
       </c>
       <c r="L63" t="s" s="2">
-        <v>96</v>
+        <v>422</v>
       </c>
       <c r="M63" t="s" s="2">
-        <v>162</v>
+        <v>423</v>
       </c>
       <c r="N63" t="s" s="2">
-        <v>98</v>
+        <v>424</v>
       </c>
       <c r="O63" s="2"/>
       <c r="P63" t="s" s="2">
@@ -9129,19 +9181,19 @@
         <v>37</v>
       </c>
       <c r="AB63" t="s" s="2">
-        <v>99</v>
+        <v>37</v>
       </c>
       <c r="AC63" t="s" s="2">
-        <v>100</v>
+        <v>37</v>
       </c>
       <c r="AD63" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AE63" t="s" s="2">
-        <v>101</v>
+        <v>37</v>
       </c>
       <c r="AF63" t="s" s="2">
-        <v>163</v>
+        <v>420</v>
       </c>
       <c r="AG63" t="s" s="2">
         <v>35</v>
@@ -9153,16 +9205,16 @@
         <v>59</v>
       </c>
       <c r="AJ63" t="s" s="2">
-        <v>103</v>
+        <v>60</v>
       </c>
       <c r="AK63" t="s" s="2">
-        <v>37</v>
+        <v>425</v>
       </c>
       <c r="AL63" t="s" s="2">
-        <v>37</v>
+        <v>61</v>
       </c>
       <c r="AM63" t="s" s="2">
-        <v>61</v>
+        <v>426</v>
       </c>
       <c r="AN63" t="s" s="2">
         <v>37</v>
@@ -9173,14 +9225,14 @@
     </row>
     <row r="64" hidden="true">
       <c r="A64" t="s" s="2">
-        <v>420</v>
+        <v>427</v>
       </c>
       <c r="B64" t="s" s="2">
-        <v>420</v>
+        <v>427</v>
       </c>
       <c r="C64" s="2"/>
       <c r="D64" t="s" s="2">
-        <v>421</v>
+        <v>37</v>
       </c>
       <c r="E64" s="2"/>
       <c r="F64" t="s" s="2">
@@ -9193,26 +9245,22 @@
         <v>37</v>
       </c>
       <c r="I64" t="s" s="2">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="J64" t="s" s="2">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="K64" t="s" s="2">
-        <v>95</v>
+        <v>428</v>
       </c>
       <c r="L64" t="s" s="2">
-        <v>422</v>
+        <v>429</v>
       </c>
       <c r="M64" t="s" s="2">
-        <v>423</v>
-      </c>
-      <c r="N64" t="s" s="2">
-        <v>98</v>
-      </c>
-      <c r="O64" t="s" s="2">
-        <v>137</v>
-      </c>
+        <v>430</v>
+      </c>
+      <c r="N64" s="2"/>
+      <c r="O64" s="2"/>
       <c r="P64" t="s" s="2">
         <v>37</v>
       </c>
@@ -9260,7 +9308,7 @@
         <v>37</v>
       </c>
       <c r="AF64" t="s" s="2">
-        <v>424</v>
+        <v>427</v>
       </c>
       <c r="AG64" t="s" s="2">
         <v>35</v>
@@ -9272,19 +9320,19 @@
         <v>59</v>
       </c>
       <c r="AJ64" t="s" s="2">
-        <v>103</v>
+        <v>60</v>
       </c>
       <c r="AK64" t="s" s="2">
-        <v>37</v>
+        <v>431</v>
       </c>
       <c r="AL64" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AM64" t="s" s="2">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="AN64" t="s" s="2">
-        <v>37</v>
+        <v>432</v>
       </c>
       <c r="AO64" t="s" s="2">
         <v>37</v>
@@ -9292,10 +9340,10 @@
     </row>
     <row r="65" hidden="true">
       <c r="A65" t="s" s="2">
-        <v>425</v>
+        <v>433</v>
       </c>
       <c r="B65" t="s" s="2">
-        <v>425</v>
+        <v>433</v>
       </c>
       <c r="C65" s="2"/>
       <c r="D65" t="s" s="2">
@@ -9303,7 +9351,7 @@
       </c>
       <c r="E65" s="2"/>
       <c r="F65" t="s" s="2">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="G65" t="s" s="2">
         <v>47</v>
@@ -9321,14 +9369,12 @@
         <v>156</v>
       </c>
       <c r="L65" t="s" s="2">
-        <v>426</v>
+        <v>157</v>
       </c>
       <c r="M65" t="s" s="2">
-        <v>427</v>
-      </c>
-      <c r="N65" t="s" s="2">
-        <v>242</v>
-      </c>
+        <v>158</v>
+      </c>
+      <c r="N65" s="2"/>
       <c r="O65" s="2"/>
       <c r="P65" t="s" s="2">
         <v>37</v>
@@ -9377,22 +9423,22 @@
         <v>37</v>
       </c>
       <c r="AF65" t="s" s="2">
-        <v>425</v>
+        <v>159</v>
       </c>
       <c r="AG65" t="s" s="2">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="AH65" t="s" s="2">
         <v>47</v>
       </c>
       <c r="AI65" t="s" s="2">
-        <v>59</v>
+        <v>37</v>
       </c>
       <c r="AJ65" t="s" s="2">
-        <v>60</v>
+        <v>37</v>
       </c>
       <c r="AK65" t="s" s="2">
-        <v>428</v>
+        <v>37</v>
       </c>
       <c r="AL65" t="s" s="2">
         <v>37</v>
@@ -9401,7 +9447,7 @@
         <v>68</v>
       </c>
       <c r="AN65" t="s" s="2">
-        <v>429</v>
+        <v>37</v>
       </c>
       <c r="AO65" t="s" s="2">
         <v>37</v>
@@ -9409,21 +9455,21 @@
     </row>
     <row r="66" hidden="true">
       <c r="A66" t="s" s="2">
-        <v>430</v>
+        <v>434</v>
       </c>
       <c r="B66" t="s" s="2">
-        <v>430</v>
+        <v>434</v>
       </c>
       <c r="C66" s="2"/>
       <c r="D66" t="s" s="2">
-        <v>37</v>
+        <v>94</v>
       </c>
       <c r="E66" s="2"/>
       <c r="F66" t="s" s="2">
         <v>35</v>
       </c>
       <c r="G66" t="s" s="2">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="H66" t="s" s="2">
         <v>37</v>
@@ -9435,16 +9481,16 @@
         <v>37</v>
       </c>
       <c r="K66" t="s" s="2">
-        <v>178</v>
+        <v>95</v>
       </c>
       <c r="L66" t="s" s="2">
-        <v>431</v>
+        <v>96</v>
       </c>
       <c r="M66" t="s" s="2">
-        <v>432</v>
+        <v>162</v>
       </c>
       <c r="N66" t="s" s="2">
-        <v>272</v>
+        <v>98</v>
       </c>
       <c r="O66" s="2"/>
       <c r="P66" t="s" s="2">
@@ -9482,43 +9528,43 @@
         <v>37</v>
       </c>
       <c r="AB66" t="s" s="2">
-        <v>37</v>
+        <v>99</v>
       </c>
       <c r="AC66" t="s" s="2">
-        <v>37</v>
+        <v>100</v>
       </c>
       <c r="AD66" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AE66" t="s" s="2">
-        <v>37</v>
+        <v>101</v>
       </c>
       <c r="AF66" t="s" s="2">
-        <v>430</v>
+        <v>163</v>
       </c>
       <c r="AG66" t="s" s="2">
         <v>35</v>
       </c>
       <c r="AH66" t="s" s="2">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="AI66" t="s" s="2">
         <v>59</v>
       </c>
       <c r="AJ66" t="s" s="2">
-        <v>60</v>
+        <v>103</v>
       </c>
       <c r="AK66" t="s" s="2">
-        <v>433</v>
+        <v>37</v>
       </c>
       <c r="AL66" t="s" s="2">
-        <v>276</v>
+        <v>37</v>
       </c>
       <c r="AM66" t="s" s="2">
-        <v>277</v>
+        <v>61</v>
       </c>
       <c r="AN66" t="s" s="2">
-        <v>434</v>
+        <v>37</v>
       </c>
       <c r="AO66" t="s" s="2">
         <v>37</v>
@@ -9533,37 +9579,39 @@
       </c>
       <c r="C67" s="2"/>
       <c r="D67" t="s" s="2">
-        <v>37</v>
+        <v>436</v>
       </c>
       <c r="E67" s="2"/>
       <c r="F67" t="s" s="2">
         <v>35</v>
       </c>
       <c r="G67" t="s" s="2">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="H67" t="s" s="2">
         <v>37</v>
       </c>
       <c r="I67" t="s" s="2">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="J67" t="s" s="2">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="K67" t="s" s="2">
-        <v>156</v>
+        <v>95</v>
       </c>
       <c r="L67" t="s" s="2">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="M67" t="s" s="2">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="N67" t="s" s="2">
-        <v>242</v>
-      </c>
-      <c r="O67" s="2"/>
+        <v>98</v>
+      </c>
+      <c r="O67" t="s" s="2">
+        <v>137</v>
+      </c>
       <c r="P67" t="s" s="2">
         <v>37</v>
       </c>
@@ -9611,31 +9659,31 @@
         <v>37</v>
       </c>
       <c r="AF67" t="s" s="2">
-        <v>435</v>
+        <v>439</v>
       </c>
       <c r="AG67" t="s" s="2">
         <v>35</v>
       </c>
       <c r="AH67" t="s" s="2">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="AI67" t="s" s="2">
         <v>59</v>
       </c>
       <c r="AJ67" t="s" s="2">
-        <v>60</v>
+        <v>103</v>
       </c>
       <c r="AK67" t="s" s="2">
-        <v>438</v>
+        <v>37</v>
       </c>
       <c r="AL67" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AM67" t="s" s="2">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="AN67" t="s" s="2">
-        <v>439</v>
+        <v>37</v>
       </c>
       <c r="AO67" t="s" s="2">
         <v>37</v>
@@ -9654,10 +9702,10 @@
       </c>
       <c r="E68" s="2"/>
       <c r="F68" t="s" s="2">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="G68" t="s" s="2">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="H68" t="s" s="2">
         <v>37</v>
@@ -9669,7 +9717,7 @@
         <v>37</v>
       </c>
       <c r="K68" t="s" s="2">
-        <v>413</v>
+        <v>156</v>
       </c>
       <c r="L68" t="s" s="2">
         <v>441</v>
@@ -9677,7 +9725,9 @@
       <c r="M68" t="s" s="2">
         <v>442</v>
       </c>
-      <c r="N68" s="2"/>
+      <c r="N68" t="s" s="2">
+        <v>242</v>
+      </c>
       <c r="O68" s="2"/>
       <c r="P68" t="s" s="2">
         <v>37</v>
@@ -9729,10 +9779,10 @@
         <v>440</v>
       </c>
       <c r="AG68" t="s" s="2">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="AH68" t="s" s="2">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="AI68" t="s" s="2">
         <v>59</v>
@@ -9750,7 +9800,7 @@
         <v>68</v>
       </c>
       <c r="AN68" t="s" s="2">
-        <v>37</v>
+        <v>444</v>
       </c>
       <c r="AO68" t="s" s="2">
         <v>37</v>
@@ -9758,10 +9808,10 @@
     </row>
     <row r="69" hidden="true">
       <c r="A69" t="s" s="2">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="B69" t="s" s="2">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="C69" s="2"/>
       <c r="D69" t="s" s="2">
@@ -9784,15 +9834,17 @@
         <v>37</v>
       </c>
       <c r="K69" t="s" s="2">
-        <v>156</v>
+        <v>178</v>
       </c>
       <c r="L69" t="s" s="2">
-        <v>157</v>
+        <v>446</v>
       </c>
       <c r="M69" t="s" s="2">
-        <v>158</v>
-      </c>
-      <c r="N69" s="2"/>
+        <v>447</v>
+      </c>
+      <c r="N69" t="s" s="2">
+        <v>272</v>
+      </c>
       <c r="O69" s="2"/>
       <c r="P69" t="s" s="2">
         <v>37</v>
@@ -9841,7 +9893,7 @@
         <v>37</v>
       </c>
       <c r="AF69" t="s" s="2">
-        <v>159</v>
+        <v>445</v>
       </c>
       <c r="AG69" t="s" s="2">
         <v>35</v>
@@ -9850,22 +9902,22 @@
         <v>47</v>
       </c>
       <c r="AI69" t="s" s="2">
-        <v>37</v>
+        <v>59</v>
       </c>
       <c r="AJ69" t="s" s="2">
-        <v>37</v>
+        <v>60</v>
       </c>
       <c r="AK69" t="s" s="2">
-        <v>37</v>
+        <v>448</v>
       </c>
       <c r="AL69" t="s" s="2">
-        <v>37</v>
+        <v>276</v>
       </c>
       <c r="AM69" t="s" s="2">
-        <v>68</v>
+        <v>277</v>
       </c>
       <c r="AN69" t="s" s="2">
-        <v>37</v>
+        <v>449</v>
       </c>
       <c r="AO69" t="s" s="2">
         <v>37</v>
@@ -9873,21 +9925,21 @@
     </row>
     <row r="70" hidden="true">
       <c r="A70" t="s" s="2">
-        <v>445</v>
+        <v>450</v>
       </c>
       <c r="B70" t="s" s="2">
-        <v>445</v>
+        <v>450</v>
       </c>
       <c r="C70" s="2"/>
       <c r="D70" t="s" s="2">
-        <v>94</v>
+        <v>37</v>
       </c>
       <c r="E70" s="2"/>
       <c r="F70" t="s" s="2">
         <v>35</v>
       </c>
       <c r="G70" t="s" s="2">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="H70" t="s" s="2">
         <v>37</v>
@@ -9899,16 +9951,16 @@
         <v>37</v>
       </c>
       <c r="K70" t="s" s="2">
-        <v>95</v>
+        <v>156</v>
       </c>
       <c r="L70" t="s" s="2">
-        <v>96</v>
+        <v>451</v>
       </c>
       <c r="M70" t="s" s="2">
-        <v>162</v>
+        <v>452</v>
       </c>
       <c r="N70" t="s" s="2">
-        <v>98</v>
+        <v>242</v>
       </c>
       <c r="O70" s="2"/>
       <c r="P70" t="s" s="2">
@@ -9946,43 +9998,43 @@
         <v>37</v>
       </c>
       <c r="AB70" t="s" s="2">
-        <v>99</v>
+        <v>37</v>
       </c>
       <c r="AC70" t="s" s="2">
-        <v>100</v>
+        <v>37</v>
       </c>
       <c r="AD70" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AE70" t="s" s="2">
-        <v>101</v>
+        <v>37</v>
       </c>
       <c r="AF70" t="s" s="2">
-        <v>163</v>
+        <v>450</v>
       </c>
       <c r="AG70" t="s" s="2">
         <v>35</v>
       </c>
       <c r="AH70" t="s" s="2">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="AI70" t="s" s="2">
         <v>59</v>
       </c>
       <c r="AJ70" t="s" s="2">
-        <v>103</v>
+        <v>60</v>
       </c>
       <c r="AK70" t="s" s="2">
-        <v>37</v>
+        <v>453</v>
       </c>
       <c r="AL70" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AM70" t="s" s="2">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="AN70" t="s" s="2">
-        <v>37</v>
+        <v>454</v>
       </c>
       <c r="AO70" t="s" s="2">
         <v>37</v>
@@ -9990,14 +10042,14 @@
     </row>
     <row r="71" hidden="true">
       <c r="A71" t="s" s="2">
-        <v>446</v>
+        <v>455</v>
       </c>
       <c r="B71" t="s" s="2">
-        <v>446</v>
+        <v>455</v>
       </c>
       <c r="C71" s="2"/>
       <c r="D71" t="s" s="2">
-        <v>421</v>
+        <v>37</v>
       </c>
       <c r="E71" s="2"/>
       <c r="F71" t="s" s="2">
@@ -10010,26 +10062,22 @@
         <v>37</v>
       </c>
       <c r="I71" t="s" s="2">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="J71" t="s" s="2">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="K71" t="s" s="2">
-        <v>95</v>
+        <v>428</v>
       </c>
       <c r="L71" t="s" s="2">
-        <v>422</v>
+        <v>456</v>
       </c>
       <c r="M71" t="s" s="2">
-        <v>423</v>
-      </c>
-      <c r="N71" t="s" s="2">
-        <v>98</v>
-      </c>
-      <c r="O71" t="s" s="2">
-        <v>137</v>
-      </c>
+        <v>457</v>
+      </c>
+      <c r="N71" s="2"/>
+      <c r="O71" s="2"/>
       <c r="P71" t="s" s="2">
         <v>37</v>
       </c>
@@ -10077,7 +10125,7 @@
         <v>37</v>
       </c>
       <c r="AF71" t="s" s="2">
-        <v>424</v>
+        <v>455</v>
       </c>
       <c r="AG71" t="s" s="2">
         <v>35</v>
@@ -10089,16 +10137,16 @@
         <v>59</v>
       </c>
       <c r="AJ71" t="s" s="2">
-        <v>103</v>
+        <v>60</v>
       </c>
       <c r="AK71" t="s" s="2">
-        <v>37</v>
+        <v>458</v>
       </c>
       <c r="AL71" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AM71" t="s" s="2">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="AN71" t="s" s="2">
         <v>37</v>
@@ -10109,10 +10157,10 @@
     </row>
     <row r="72" hidden="true">
       <c r="A72" t="s" s="2">
-        <v>447</v>
+        <v>459</v>
       </c>
       <c r="B72" t="s" s="2">
-        <v>447</v>
+        <v>459</v>
       </c>
       <c r="C72" s="2"/>
       <c r="D72" t="s" s="2">
@@ -10138,14 +10186,12 @@
         <v>156</v>
       </c>
       <c r="L72" t="s" s="2">
-        <v>448</v>
+        <v>157</v>
       </c>
       <c r="M72" t="s" s="2">
-        <v>449</v>
-      </c>
-      <c r="N72" t="s" s="2">
-        <v>242</v>
-      </c>
+        <v>158</v>
+      </c>
+      <c r="N72" s="2"/>
       <c r="O72" s="2"/>
       <c r="P72" t="s" s="2">
         <v>37</v>
@@ -10194,7 +10240,7 @@
         <v>37</v>
       </c>
       <c r="AF72" t="s" s="2">
-        <v>447</v>
+        <v>159</v>
       </c>
       <c r="AG72" t="s" s="2">
         <v>35</v>
@@ -10203,13 +10249,13 @@
         <v>47</v>
       </c>
       <c r="AI72" t="s" s="2">
-        <v>59</v>
+        <v>37</v>
       </c>
       <c r="AJ72" t="s" s="2">
-        <v>60</v>
+        <v>37</v>
       </c>
       <c r="AK72" t="s" s="2">
-        <v>450</v>
+        <v>37</v>
       </c>
       <c r="AL72" t="s" s="2">
         <v>37</v>
@@ -10226,21 +10272,21 @@
     </row>
     <row r="73" hidden="true">
       <c r="A73" t="s" s="2">
-        <v>451</v>
+        <v>460</v>
       </c>
       <c r="B73" t="s" s="2">
-        <v>451</v>
+        <v>460</v>
       </c>
       <c r="C73" s="2"/>
       <c r="D73" t="s" s="2">
-        <v>37</v>
+        <v>94</v>
       </c>
       <c r="E73" s="2"/>
       <c r="F73" t="s" s="2">
         <v>35</v>
       </c>
       <c r="G73" t="s" s="2">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="H73" t="s" s="2">
         <v>37</v>
@@ -10252,16 +10298,16 @@
         <v>37</v>
       </c>
       <c r="K73" t="s" s="2">
-        <v>178</v>
+        <v>95</v>
       </c>
       <c r="L73" t="s" s="2">
-        <v>452</v>
+        <v>96</v>
       </c>
       <c r="M73" t="s" s="2">
-        <v>453</v>
+        <v>162</v>
       </c>
       <c r="N73" t="s" s="2">
-        <v>272</v>
+        <v>98</v>
       </c>
       <c r="O73" s="2"/>
       <c r="P73" t="s" s="2">
@@ -10287,62 +10333,415 @@
         <v>37</v>
       </c>
       <c r="X73" t="s" s="2">
-        <v>74</v>
+        <v>37</v>
       </c>
       <c r="Y73" t="s" s="2">
-        <v>454</v>
+        <v>37</v>
       </c>
       <c r="Z73" t="s" s="2">
-        <v>455</v>
+        <v>37</v>
       </c>
       <c r="AA73" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AB73" t="s" s="2">
-        <v>37</v>
+        <v>99</v>
       </c>
       <c r="AC73" t="s" s="2">
-        <v>37</v>
+        <v>100</v>
       </c>
       <c r="AD73" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AE73" t="s" s="2">
-        <v>37</v>
+        <v>101</v>
       </c>
       <c r="AF73" t="s" s="2">
-        <v>451</v>
+        <v>163</v>
       </c>
       <c r="AG73" t="s" s="2">
         <v>35</v>
       </c>
       <c r="AH73" t="s" s="2">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="AI73" t="s" s="2">
         <v>59</v>
       </c>
       <c r="AJ73" t="s" s="2">
+        <v>103</v>
+      </c>
+      <c r="AK73" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AL73" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AM73" t="s" s="2">
+        <v>61</v>
+      </c>
+      <c r="AN73" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AO73" t="s" s="2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="74" hidden="true">
+      <c r="A74" t="s" s="2">
+        <v>461</v>
+      </c>
+      <c r="B74" t="s" s="2">
+        <v>461</v>
+      </c>
+      <c r="C74" s="2"/>
+      <c r="D74" t="s" s="2">
+        <v>436</v>
+      </c>
+      <c r="E74" s="2"/>
+      <c r="F74" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="G74" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="H74" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="I74" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="J74" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="K74" t="s" s="2">
+        <v>95</v>
+      </c>
+      <c r="L74" t="s" s="2">
+        <v>437</v>
+      </c>
+      <c r="M74" t="s" s="2">
+        <v>438</v>
+      </c>
+      <c r="N74" t="s" s="2">
+        <v>98</v>
+      </c>
+      <c r="O74" t="s" s="2">
+        <v>137</v>
+      </c>
+      <c r="P74" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="Q74" s="2"/>
+      <c r="R74" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="S74" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="T74" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="U74" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="V74" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="W74" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="X74" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="Y74" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="Z74" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AA74" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AB74" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AC74" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AD74" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AE74" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AF74" t="s" s="2">
+        <v>439</v>
+      </c>
+      <c r="AG74" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AH74" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="AI74" t="s" s="2">
+        <v>59</v>
+      </c>
+      <c r="AJ74" t="s" s="2">
+        <v>103</v>
+      </c>
+      <c r="AK74" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AL74" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AM74" t="s" s="2">
+        <v>61</v>
+      </c>
+      <c r="AN74" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AO74" t="s" s="2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="75" hidden="true">
+      <c r="A75" t="s" s="2">
+        <v>462</v>
+      </c>
+      <c r="B75" t="s" s="2">
+        <v>462</v>
+      </c>
+      <c r="C75" s="2"/>
+      <c r="D75" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="E75" s="2"/>
+      <c r="F75" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="G75" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="H75" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="I75" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="J75" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="K75" t="s" s="2">
+        <v>156</v>
+      </c>
+      <c r="L75" t="s" s="2">
+        <v>463</v>
+      </c>
+      <c r="M75" t="s" s="2">
+        <v>464</v>
+      </c>
+      <c r="N75" t="s" s="2">
+        <v>242</v>
+      </c>
+      <c r="O75" s="2"/>
+      <c r="P75" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="Q75" s="2"/>
+      <c r="R75" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="S75" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="T75" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="U75" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="V75" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="W75" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="X75" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="Y75" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="Z75" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AA75" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AB75" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AC75" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AD75" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AE75" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AF75" t="s" s="2">
+        <v>462</v>
+      </c>
+      <c r="AG75" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AH75" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="AI75" t="s" s="2">
+        <v>59</v>
+      </c>
+      <c r="AJ75" t="s" s="2">
         <v>60</v>
       </c>
-      <c r="AK73" t="s" s="2">
-        <v>456</v>
-      </c>
-      <c r="AL73" t="s" s="2">
+      <c r="AK75" t="s" s="2">
+        <v>465</v>
+      </c>
+      <c r="AL75" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AM75" t="s" s="2">
+        <v>68</v>
+      </c>
+      <c r="AN75" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AO75" t="s" s="2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="76" hidden="true">
+      <c r="A76" t="s" s="2">
+        <v>466</v>
+      </c>
+      <c r="B76" t="s" s="2">
+        <v>466</v>
+      </c>
+      <c r="C76" s="2"/>
+      <c r="D76" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="E76" s="2"/>
+      <c r="F76" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="G76" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="H76" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="I76" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="J76" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="K76" t="s" s="2">
+        <v>178</v>
+      </c>
+      <c r="L76" t="s" s="2">
+        <v>467</v>
+      </c>
+      <c r="M76" t="s" s="2">
+        <v>468</v>
+      </c>
+      <c r="N76" t="s" s="2">
+        <v>272</v>
+      </c>
+      <c r="O76" s="2"/>
+      <c r="P76" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="Q76" s="2"/>
+      <c r="R76" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="S76" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="T76" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="U76" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="V76" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="W76" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="X76" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="Y76" t="s" s="2">
+        <v>469</v>
+      </c>
+      <c r="Z76" t="s" s="2">
+        <v>470</v>
+      </c>
+      <c r="AA76" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AB76" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AC76" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AD76" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AE76" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AF76" t="s" s="2">
+        <v>466</v>
+      </c>
+      <c r="AG76" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AH76" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="AI76" t="s" s="2">
+        <v>59</v>
+      </c>
+      <c r="AJ76" t="s" s="2">
+        <v>60</v>
+      </c>
+      <c r="AK76" t="s" s="2">
+        <v>471</v>
+      </c>
+      <c r="AL76" t="s" s="2">
         <v>276</v>
       </c>
-      <c r="AM73" t="s" s="2">
+      <c r="AM76" t="s" s="2">
         <v>277</v>
       </c>
-      <c r="AN73" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AO73" t="s" s="2">
+      <c r="AN76" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AO76" t="s" s="2">
         <v>37</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AO73">
+  <autoFilter ref="A1:AO76">
     <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -10352,7 +10751,7 @@
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>
-  <conditionalFormatting sqref="A2:AI72">
+  <conditionalFormatting sqref="A2:AI75">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$G2&lt;&gt;"Y"</formula>
     </cfRule>

</xml_diff>

<commit_message>
Sd creation de code systems study population regulation code reglementation precision (#72)
* ajout CS et VS

* add eclaire-category-vs et binding 3d8dd35cf90a033723d9ebf05f658d3eb3a71609
</commit_message>
<xml_diff>
--- a/ig/main/StructureDefinition-eclaire-researchstudy.xlsx
+++ b/ig/main/StructureDefinition-eclaire-researchstudy.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3184" uniqueCount="504">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3183" uniqueCount="504">
   <si>
     <t>Property</t>
   </si>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-10-14T10:16:45+00:00</t>
+    <t>2023-10-14T10:31:55+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -900,25 +900,25 @@
     <t>Codes categorizing the type of study such as investigational vs. observational, type of blinding, type of randomization, safety vs. efficacy, etc.</t>
   </si>
   <si>
+    <t>https://interop.esante.gouv.fr/ig/fhir/eclaire/ValueSet/eclaire-category-vs</t>
+  </si>
+  <si>
+    <t>InterventionalStudyProtocolVersion; InterventionalStudyProtocol.allocationCode; InterventionalStudyProtocol.blindedRoleCode; InterventionalStudyProtocol.blindingSchemaCode; InterventionalStudyProtocol.controlTypeCode</t>
+  </si>
+  <si>
+    <t>Study Type; Primary Purpose; Interventional Model; Masking; Allocation; study Classification; Observational Study Model; Time Perspective; Biospecimen Retention</t>
+  </si>
+  <si>
+    <t>ResearchStudy.focus</t>
+  </si>
+  <si>
+    <t>Drugs, devices, etc. under study</t>
+  </si>
+  <si>
+    <t>The medication(s), food(s), therapy(ies), device(s) or other concerns or interventions that the study is seeking to gain more information about.</t>
+  </si>
+  <si>
     <t>example</t>
-  </si>
-  <si>
-    <t>Codes that describe the type of research study.  E.g. Study phase, Interventional/Observational, blinding type, etc.</t>
-  </si>
-  <si>
-    <t>InterventionalStudyProtocolVersion; InterventionalStudyProtocol.allocationCode; InterventionalStudyProtocol.blindedRoleCode; InterventionalStudyProtocol.blindingSchemaCode; InterventionalStudyProtocol.controlTypeCode</t>
-  </si>
-  <si>
-    <t>Study Type; Primary Purpose; Interventional Model; Masking; Allocation; study Classification; Observational Study Model; Time Perspective; Biospecimen Retention</t>
-  </si>
-  <si>
-    <t>ResearchStudy.focus</t>
-  </si>
-  <si>
-    <t>Drugs, devices, etc. under study</t>
-  </si>
-  <si>
-    <t>The medication(s), food(s), therapy(ies), device(s) or other concerns or interventions that the study is seeking to gain more information about.</t>
   </si>
   <si>
     <t>Codes for medications, devices and other interventions.</t>
@@ -1924,7 +1924,7 @@
     <col min="22" max="22" width="1.04296875" customWidth="true" bestFit="true"/>
     <col min="23" max="23" width="1.04296875" customWidth="true" bestFit="true"/>
     <col min="24" max="24" width="10.53125" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="106.69140625" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="98.375" customWidth="true" bestFit="true"/>
     <col min="26" max="26" width="71.046875" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="1.04296875" customWidth="true" bestFit="true"/>
     <col min="28" max="28" width="11.08203125" customWidth="true" bestFit="true"/>
@@ -6581,13 +6581,11 @@
         <v>37</v>
       </c>
       <c r="X40" t="s" s="2">
+        <v>178</v>
+      </c>
+      <c r="Y40" s="2"/>
+      <c r="Z40" t="s" s="2">
         <v>282</v>
-      </c>
-      <c r="Y40" t="s" s="2">
-        <v>283</v>
-      </c>
-      <c r="Z40" t="s" s="2">
-        <v>37</v>
       </c>
       <c r="AA40" t="s" s="2">
         <v>37</v>
@@ -6620,7 +6618,7 @@
         <v>60</v>
       </c>
       <c r="AK40" t="s" s="2">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="AL40" t="s" s="2">
         <v>271</v>
@@ -6629,7 +6627,7 @@
         <v>272</v>
       </c>
       <c r="AN40" t="s" s="2">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="AO40" t="s" s="2">
         <v>37</v>
@@ -6637,10 +6635,10 @@
     </row>
     <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B41" t="s" s="2">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C41" s="2"/>
       <c r="D41" t="s" s="2">
@@ -6666,10 +6664,10 @@
         <v>173</v>
       </c>
       <c r="L41" t="s" s="2">
+        <v>286</v>
+      </c>
+      <c r="M41" t="s" s="2">
         <v>287</v>
-      </c>
-      <c r="M41" t="s" s="2">
-        <v>288</v>
       </c>
       <c r="N41" t="s" s="2">
         <v>267</v>
@@ -6698,7 +6696,7 @@
         <v>37</v>
       </c>
       <c r="X41" t="s" s="2">
-        <v>282</v>
+        <v>288</v>
       </c>
       <c r="Y41" t="s" s="2">
         <v>289</v>
@@ -6722,7 +6720,7 @@
         <v>37</v>
       </c>
       <c r="AF41" t="s" s="2">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="AG41" t="s" s="2">
         <v>35</v>
@@ -6815,7 +6813,7 @@
         <v>37</v>
       </c>
       <c r="X42" t="s" s="2">
-        <v>282</v>
+        <v>288</v>
       </c>
       <c r="Y42" t="s" s="2">
         <v>296</v>
@@ -6934,7 +6932,7 @@
         <v>37</v>
       </c>
       <c r="X43" t="s" s="2">
-        <v>282</v>
+        <v>288</v>
       </c>
       <c r="Y43" t="s" s="2">
         <v>296</v>
@@ -7523,7 +7521,7 @@
         <v>37</v>
       </c>
       <c r="X48" t="s" s="2">
-        <v>282</v>
+        <v>288</v>
       </c>
       <c r="Y48" t="s" s="2">
         <v>296</v>
@@ -9274,7 +9272,7 @@
         <v>37</v>
       </c>
       <c r="X63" t="s" s="2">
-        <v>282</v>
+        <v>288</v>
       </c>
       <c r="Y63" t="s" s="2">
         <v>388</v>
@@ -10210,7 +10208,7 @@
         <v>37</v>
       </c>
       <c r="X71" t="s" s="2">
-        <v>282</v>
+        <v>288</v>
       </c>
       <c r="Y71" t="s" s="2">
         <v>447</v>

</xml_diff>

<commit_message>
Sd ref profils (#103)
* add contraintes ref

* Update ECLAIREResearchStudy.fsh c7a0700ddac2512a33d6093ecaeb872fc47e773e
</commit_message>
<xml_diff>
--- a/ig/main/StructureDefinition-eclaire-researchstudy.xlsx
+++ b/ig/main/StructureDefinition-eclaire-researchstudy.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-11-13T14:27:10+00:00</t>
+    <t>2023-12-23T14:24:05+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -1555,7 +1555,7 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(Group)
+    <t xml:space="preserve">Reference(https://interop.esante.gouv.fr/ig/fhir/eclaire/StructureDefinition/eclaire-group)
 </t>
   </si>
   <si>
@@ -1654,7 +1654,7 @@
     <t>ResearchStudy.site</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(Location)
+    <t xml:space="preserve">Reference(https://interop.esante.gouv.fr/ig/fhir/eclaire/StructureDefinition/eclaire-location)
 </t>
   </si>
   <si>

</xml_diff>

<commit_message>
add short relatedArtifact (#114)
* add short relatedArtifact 0d87240a78f138e1d743647c712df95c00bd3a35
</commit_message>
<xml_diff>
--- a/ig/main/StructureDefinition-eclaire-researchstudy.xlsx
+++ b/ig/main/StructureDefinition-eclaire-researchstudy.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-01-11T09:08:43+00:00</t>
+    <t>2024-01-11T11:17:12+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -1475,7 +1475,7 @@
 </t>
   </si>
   <si>
-    <t>References and dependencies</t>
+    <t>Publications et résumé des résultats / Publications about the study and Summary results</t>
   </si>
   <si>
     <t>Citations, references and other related documents.</t>
@@ -10341,7 +10341,7 @@
         <v>79</v>
       </c>
       <c r="H70" t="s" s="2">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="I70" t="s" s="2">
         <v>80</v>

</xml_diff>

<commit_message>
ajout completion date (#116)
* ajout completion date

* MaJ mapping completion date

---------

Co-authored-by: sly-kereval <125375447+sly-kereval@users.noreply.github.com> 1ebb592ce940d2e3f4a1c9ce7f545b69c0b66162
</commit_message>
<xml_diff>
--- a/ig/main/StructureDefinition-eclaire-researchstudy.xlsx
+++ b/ig/main/StructureDefinition-eclaire-researchstudy.xlsx
@@ -10,13 +10,13 @@
     <sheet name="Elements" r:id="rId4" sheetId="2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="true">Elements!$A$1:$AO$93</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="true">Elements!$A$1:$AO$97</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3488" uniqueCount="594">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3636" uniqueCount="613">
   <si>
     <t>Property</t>
   </si>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-01-15T15:15:33+00:00</t>
+    <t>2024-01-22T13:46:22+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -1606,6 +1606,65 @@
   </si>
   <si>
     <t>FiveWs.done[x]</t>
+  </si>
+  <si>
+    <t>ResearchStudy.period.id</t>
+  </si>
+  <si>
+    <t>ResearchStudy.period.extension</t>
+  </si>
+  <si>
+    <t>ResearchStudy.period.start</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dateTime
+</t>
+  </si>
+  <si>
+    <t>Starting time with inclusive boundary</t>
+  </si>
+  <si>
+    <t>The start of the period. The boundary is inclusive.</t>
+  </si>
+  <si>
+    <t>If the low element is missing, the meaning is that the low boundary is not known.</t>
+  </si>
+  <si>
+    <t>Period.start</t>
+  </si>
+  <si>
+    <t>ele-1
+per-1</t>
+  </si>
+  <si>
+    <t>DR.1</t>
+  </si>
+  <si>
+    <t>./low</t>
+  </si>
+  <si>
+    <t>ResearchStudy.period.end</t>
+  </si>
+  <si>
+    <t>Date à laquelle l'essai se termine (la date initiale est prévisionnelle) / Completion date</t>
+  </si>
+  <si>
+    <t>The end of the period. If the end of the period is missing, it means no end was known or planned at the time the instance was created. The start may be in the past, and the end date in the future, which means that period is expected/planned to end at that time.</t>
+  </si>
+  <si>
+    <t>The high value includes any matching date/time. i.e. 2012-02-03T10:00:00 is in a period that has an end value of 2012-02-03.</t>
+  </si>
+  <si>
+    <t>If the end of the period is missing, it means that the period is ongoing</t>
+  </si>
+  <si>
+    <t>Period.end</t>
+  </si>
+  <si>
+    <t>DR.2</t>
+  </si>
+  <si>
+    <t>./high</t>
   </si>
   <si>
     <t>ResearchStudy.sponsor</t>
@@ -2172,7 +2231,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AO93"/>
+  <dimension ref="A1:AO97"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -11043,26 +11102,24 @@
         <v>90</v>
       </c>
       <c r="H76" t="s" s="2">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="I76" t="s" s="2">
         <v>80</v>
       </c>
       <c r="J76" t="s" s="2">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="K76" t="s" s="2">
-        <v>257</v>
+        <v>194</v>
       </c>
       <c r="L76" t="s" s="2">
-        <v>514</v>
+        <v>195</v>
       </c>
       <c r="M76" t="s" s="2">
-        <v>515</v>
-      </c>
-      <c r="N76" t="s" s="2">
-        <v>287</v>
-      </c>
+        <v>196</v>
+      </c>
+      <c r="N76" s="2"/>
       <c r="O76" s="2"/>
       <c r="P76" t="s" s="2">
         <v>80</v>
@@ -11111,7 +11168,7 @@
         <v>80</v>
       </c>
       <c r="AF76" t="s" s="2">
-        <v>513</v>
+        <v>197</v>
       </c>
       <c r="AG76" t="s" s="2">
         <v>78</v>
@@ -11120,44 +11177,44 @@
         <v>90</v>
       </c>
       <c r="AI76" t="s" s="2">
-        <v>102</v>
+        <v>80</v>
       </c>
       <c r="AJ76" t="s" s="2">
-        <v>262</v>
+        <v>80</v>
       </c>
       <c r="AK76" t="s" s="2">
-        <v>516</v>
+        <v>80</v>
       </c>
       <c r="AL76" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AM76" t="s" s="2">
-        <v>517</v>
+        <v>111</v>
       </c>
       <c r="AN76" t="s" s="2">
-        <v>518</v>
+        <v>80</v>
       </c>
       <c r="AO76" t="s" s="2">
-        <v>519</v>
+        <v>80</v>
       </c>
     </row>
     <row r="77" hidden="true">
       <c r="A77" t="s" s="2">
-        <v>520</v>
+        <v>514</v>
       </c>
       <c r="B77" t="s" s="2">
-        <v>520</v>
+        <v>514</v>
       </c>
       <c r="C77" s="2"/>
       <c r="D77" t="s" s="2">
-        <v>80</v>
+        <v>137</v>
       </c>
       <c r="E77" s="2"/>
       <c r="F77" t="s" s="2">
         <v>78</v>
       </c>
       <c r="G77" t="s" s="2">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="H77" t="s" s="2">
         <v>80</v>
@@ -11166,19 +11223,19 @@
         <v>80</v>
       </c>
       <c r="J77" t="s" s="2">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="K77" t="s" s="2">
-        <v>521</v>
+        <v>138</v>
       </c>
       <c r="L77" t="s" s="2">
-        <v>522</v>
+        <v>139</v>
       </c>
       <c r="M77" t="s" s="2">
-        <v>523</v>
+        <v>200</v>
       </c>
       <c r="N77" t="s" s="2">
-        <v>287</v>
+        <v>141</v>
       </c>
       <c r="O77" s="2"/>
       <c r="P77" t="s" s="2">
@@ -11216,54 +11273,54 @@
         <v>80</v>
       </c>
       <c r="AB77" t="s" s="2">
-        <v>80</v>
+        <v>142</v>
       </c>
       <c r="AC77" t="s" s="2">
-        <v>80</v>
+        <v>143</v>
       </c>
       <c r="AD77" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AE77" t="s" s="2">
-        <v>80</v>
+        <v>144</v>
       </c>
       <c r="AF77" t="s" s="2">
-        <v>520</v>
+        <v>201</v>
       </c>
       <c r="AG77" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AH77" t="s" s="2">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="AI77" t="s" s="2">
         <v>102</v>
       </c>
       <c r="AJ77" t="s" s="2">
-        <v>262</v>
+        <v>146</v>
       </c>
       <c r="AK77" t="s" s="2">
-        <v>524</v>
+        <v>80</v>
       </c>
       <c r="AL77" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AM77" t="s" s="2">
-        <v>525</v>
+        <v>104</v>
       </c>
       <c r="AN77" t="s" s="2">
-        <v>526</v>
+        <v>80</v>
       </c>
       <c r="AO77" t="s" s="2">
-        <v>519</v>
+        <v>80</v>
       </c>
     </row>
     <row r="78" hidden="true">
       <c r="A78" t="s" s="2">
-        <v>527</v>
+        <v>515</v>
       </c>
       <c r="B78" t="s" s="2">
-        <v>527</v>
+        <v>515</v>
       </c>
       <c r="C78" s="2"/>
       <c r="D78" t="s" s="2">
@@ -11274,10 +11331,10 @@
         <v>78</v>
       </c>
       <c r="G78" t="s" s="2">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="H78" t="s" s="2">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="I78" t="s" s="2">
         <v>80</v>
@@ -11286,16 +11343,16 @@
         <v>91</v>
       </c>
       <c r="K78" t="s" s="2">
-        <v>528</v>
+        <v>516</v>
       </c>
       <c r="L78" t="s" s="2">
-        <v>529</v>
+        <v>517</v>
       </c>
       <c r="M78" t="s" s="2">
-        <v>530</v>
+        <v>518</v>
       </c>
       <c r="N78" t="s" s="2">
-        <v>287</v>
+        <v>519</v>
       </c>
       <c r="O78" s="2"/>
       <c r="P78" t="s" s="2">
@@ -11345,42 +11402,42 @@
         <v>80</v>
       </c>
       <c r="AF78" t="s" s="2">
-        <v>527</v>
+        <v>520</v>
       </c>
       <c r="AG78" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AH78" t="s" s="2">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="AI78" t="s" s="2">
-        <v>102</v>
+        <v>521</v>
       </c>
       <c r="AJ78" t="s" s="2">
-        <v>262</v>
+        <v>103</v>
       </c>
       <c r="AK78" t="s" s="2">
-        <v>531</v>
+        <v>80</v>
       </c>
       <c r="AL78" t="s" s="2">
-        <v>80</v>
+        <v>522</v>
       </c>
       <c r="AM78" t="s" s="2">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="AN78" t="s" s="2">
-        <v>532</v>
+        <v>80</v>
       </c>
       <c r="AO78" t="s" s="2">
-        <v>533</v>
+        <v>80</v>
       </c>
     </row>
     <row r="79" hidden="true">
       <c r="A79" t="s" s="2">
-        <v>534</v>
+        <v>524</v>
       </c>
       <c r="B79" t="s" s="2">
-        <v>534</v>
+        <v>524</v>
       </c>
       <c r="C79" s="2"/>
       <c r="D79" t="s" s="2">
@@ -11394,7 +11451,7 @@
         <v>90</v>
       </c>
       <c r="H79" t="s" s="2">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="I79" t="s" s="2">
         <v>80</v>
@@ -11403,22 +11460,24 @@
         <v>91</v>
       </c>
       <c r="K79" t="s" s="2">
-        <v>216</v>
+        <v>516</v>
       </c>
       <c r="L79" t="s" s="2">
-        <v>535</v>
+        <v>525</v>
       </c>
       <c r="M79" t="s" s="2">
-        <v>536</v>
+        <v>526</v>
       </c>
       <c r="N79" t="s" s="2">
-        <v>310</v>
+        <v>527</v>
       </c>
       <c r="O79" s="2"/>
       <c r="P79" t="s" s="2">
         <v>80</v>
       </c>
-      <c r="Q79" s="2"/>
+      <c r="Q79" t="s" s="2">
+        <v>528</v>
+      </c>
       <c r="R79" t="s" s="2">
         <v>80</v>
       </c>
@@ -11438,13 +11497,13 @@
         <v>80</v>
       </c>
       <c r="X79" t="s" s="2">
-        <v>331</v>
+        <v>80</v>
       </c>
       <c r="Y79" t="s" s="2">
-        <v>537</v>
+        <v>80</v>
       </c>
       <c r="Z79" t="s" s="2">
-        <v>538</v>
+        <v>80</v>
       </c>
       <c r="AA79" t="s" s="2">
         <v>80</v>
@@ -11462,7 +11521,7 @@
         <v>80</v>
       </c>
       <c r="AF79" t="s" s="2">
-        <v>534</v>
+        <v>529</v>
       </c>
       <c r="AG79" t="s" s="2">
         <v>78</v>
@@ -11471,33 +11530,33 @@
         <v>90</v>
       </c>
       <c r="AI79" t="s" s="2">
-        <v>102</v>
+        <v>521</v>
       </c>
       <c r="AJ79" t="s" s="2">
         <v>103</v>
       </c>
       <c r="AK79" t="s" s="2">
-        <v>539</v>
+        <v>80</v>
       </c>
       <c r="AL79" t="s" s="2">
-        <v>314</v>
+        <v>530</v>
       </c>
       <c r="AM79" t="s" s="2">
-        <v>315</v>
+        <v>531</v>
       </c>
       <c r="AN79" t="s" s="2">
-        <v>540</v>
+        <v>80</v>
       </c>
       <c r="AO79" t="s" s="2">
-        <v>541</v>
+        <v>80</v>
       </c>
     </row>
     <row r="80" hidden="true">
       <c r="A80" t="s" s="2">
-        <v>542</v>
+        <v>532</v>
       </c>
       <c r="B80" t="s" s="2">
-        <v>542</v>
+        <v>532</v>
       </c>
       <c r="C80" s="2"/>
       <c r="D80" t="s" s="2">
@@ -11508,28 +11567,28 @@
         <v>78</v>
       </c>
       <c r="G80" t="s" s="2">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="H80" t="s" s="2">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="I80" t="s" s="2">
         <v>80</v>
       </c>
       <c r="J80" t="s" s="2">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="K80" t="s" s="2">
-        <v>543</v>
+        <v>257</v>
       </c>
       <c r="L80" t="s" s="2">
-        <v>544</v>
+        <v>533</v>
       </c>
       <c r="M80" t="s" s="2">
-        <v>545</v>
+        <v>534</v>
       </c>
       <c r="N80" t="s" s="2">
-        <v>546</v>
+        <v>287</v>
       </c>
       <c r="O80" s="2"/>
       <c r="P80" t="s" s="2">
@@ -11579,42 +11638,42 @@
         <v>80</v>
       </c>
       <c r="AF80" t="s" s="2">
-        <v>542</v>
+        <v>532</v>
       </c>
       <c r="AG80" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AH80" t="s" s="2">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="AI80" t="s" s="2">
         <v>102</v>
       </c>
       <c r="AJ80" t="s" s="2">
-        <v>103</v>
+        <v>262</v>
       </c>
       <c r="AK80" t="s" s="2">
-        <v>547</v>
+        <v>535</v>
       </c>
       <c r="AL80" t="s" s="2">
-        <v>104</v>
+        <v>80</v>
       </c>
       <c r="AM80" t="s" s="2">
-        <v>548</v>
+        <v>536</v>
       </c>
       <c r="AN80" t="s" s="2">
-        <v>80</v>
+        <v>537</v>
       </c>
       <c r="AO80" t="s" s="2">
-        <v>80</v>
+        <v>538</v>
       </c>
     </row>
     <row r="81" hidden="true">
       <c r="A81" t="s" s="2">
-        <v>549</v>
+        <v>539</v>
       </c>
       <c r="B81" t="s" s="2">
-        <v>549</v>
+        <v>539</v>
       </c>
       <c r="C81" s="2"/>
       <c r="D81" t="s" s="2">
@@ -11625,7 +11684,7 @@
         <v>78</v>
       </c>
       <c r="G81" t="s" s="2">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="H81" t="s" s="2">
         <v>80</v>
@@ -11634,18 +11693,20 @@
         <v>80</v>
       </c>
       <c r="J81" t="s" s="2">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="K81" t="s" s="2">
-        <v>550</v>
+        <v>540</v>
       </c>
       <c r="L81" t="s" s="2">
-        <v>551</v>
+        <v>541</v>
       </c>
       <c r="M81" t="s" s="2">
-        <v>552</v>
-      </c>
-      <c r="N81" s="2"/>
+        <v>542</v>
+      </c>
+      <c r="N81" t="s" s="2">
+        <v>287</v>
+      </c>
       <c r="O81" s="2"/>
       <c r="P81" t="s" s="2">
         <v>80</v>
@@ -11694,42 +11755,42 @@
         <v>80</v>
       </c>
       <c r="AF81" t="s" s="2">
-        <v>549</v>
+        <v>539</v>
       </c>
       <c r="AG81" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AH81" t="s" s="2">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="AI81" t="s" s="2">
         <v>102</v>
       </c>
       <c r="AJ81" t="s" s="2">
-        <v>103</v>
+        <v>262</v>
       </c>
       <c r="AK81" t="s" s="2">
-        <v>553</v>
+        <v>543</v>
       </c>
       <c r="AL81" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AM81" t="s" s="2">
-        <v>111</v>
+        <v>544</v>
       </c>
       <c r="AN81" t="s" s="2">
-        <v>554</v>
+        <v>545</v>
       </c>
       <c r="AO81" t="s" s="2">
-        <v>80</v>
+        <v>538</v>
       </c>
     </row>
     <row r="82" hidden="true">
       <c r="A82" t="s" s="2">
-        <v>555</v>
+        <v>546</v>
       </c>
       <c r="B82" t="s" s="2">
-        <v>555</v>
+        <v>546</v>
       </c>
       <c r="C82" s="2"/>
       <c r="D82" t="s" s="2">
@@ -11740,27 +11801,29 @@
         <v>78</v>
       </c>
       <c r="G82" t="s" s="2">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="H82" t="s" s="2">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="I82" t="s" s="2">
         <v>80</v>
       </c>
       <c r="J82" t="s" s="2">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="K82" t="s" s="2">
-        <v>194</v>
+        <v>547</v>
       </c>
       <c r="L82" t="s" s="2">
-        <v>195</v>
+        <v>548</v>
       </c>
       <c r="M82" t="s" s="2">
-        <v>196</v>
-      </c>
-      <c r="N82" s="2"/>
+        <v>549</v>
+      </c>
+      <c r="N82" t="s" s="2">
+        <v>287</v>
+      </c>
       <c r="O82" s="2"/>
       <c r="P82" t="s" s="2">
         <v>80</v>
@@ -11809,53 +11872,53 @@
         <v>80</v>
       </c>
       <c r="AF82" t="s" s="2">
-        <v>197</v>
+        <v>546</v>
       </c>
       <c r="AG82" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AH82" t="s" s="2">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="AI82" t="s" s="2">
-        <v>80</v>
+        <v>102</v>
       </c>
       <c r="AJ82" t="s" s="2">
-        <v>80</v>
+        <v>262</v>
       </c>
       <c r="AK82" t="s" s="2">
-        <v>80</v>
+        <v>550</v>
       </c>
       <c r="AL82" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AM82" t="s" s="2">
-        <v>111</v>
+        <v>544</v>
       </c>
       <c r="AN82" t="s" s="2">
-        <v>80</v>
+        <v>551</v>
       </c>
       <c r="AO82" t="s" s="2">
-        <v>80</v>
+        <v>552</v>
       </c>
     </row>
     <row r="83" hidden="true">
       <c r="A83" t="s" s="2">
-        <v>556</v>
+        <v>553</v>
       </c>
       <c r="B83" t="s" s="2">
-        <v>556</v>
+        <v>553</v>
       </c>
       <c r="C83" s="2"/>
       <c r="D83" t="s" s="2">
-        <v>137</v>
+        <v>80</v>
       </c>
       <c r="E83" s="2"/>
       <c r="F83" t="s" s="2">
         <v>78</v>
       </c>
       <c r="G83" t="s" s="2">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="H83" t="s" s="2">
         <v>80</v>
@@ -11864,19 +11927,19 @@
         <v>80</v>
       </c>
       <c r="J83" t="s" s="2">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="K83" t="s" s="2">
-        <v>138</v>
+        <v>216</v>
       </c>
       <c r="L83" t="s" s="2">
-        <v>139</v>
+        <v>554</v>
       </c>
       <c r="M83" t="s" s="2">
-        <v>200</v>
+        <v>555</v>
       </c>
       <c r="N83" t="s" s="2">
-        <v>141</v>
+        <v>310</v>
       </c>
       <c r="O83" s="2"/>
       <c r="P83" t="s" s="2">
@@ -11902,70 +11965,70 @@
         <v>80</v>
       </c>
       <c r="X83" t="s" s="2">
-        <v>80</v>
+        <v>331</v>
       </c>
       <c r="Y83" t="s" s="2">
-        <v>80</v>
+        <v>556</v>
       </c>
       <c r="Z83" t="s" s="2">
-        <v>80</v>
+        <v>557</v>
       </c>
       <c r="AA83" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AB83" t="s" s="2">
-        <v>142</v>
+        <v>80</v>
       </c>
       <c r="AC83" t="s" s="2">
-        <v>143</v>
+        <v>80</v>
       </c>
       <c r="AD83" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AE83" t="s" s="2">
-        <v>144</v>
+        <v>80</v>
       </c>
       <c r="AF83" t="s" s="2">
-        <v>201</v>
+        <v>553</v>
       </c>
       <c r="AG83" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AH83" t="s" s="2">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="AI83" t="s" s="2">
         <v>102</v>
       </c>
       <c r="AJ83" t="s" s="2">
-        <v>146</v>
+        <v>103</v>
       </c>
       <c r="AK83" t="s" s="2">
-        <v>80</v>
+        <v>558</v>
       </c>
       <c r="AL83" t="s" s="2">
-        <v>80</v>
+        <v>314</v>
       </c>
       <c r="AM83" t="s" s="2">
-        <v>104</v>
+        <v>315</v>
       </c>
       <c r="AN83" t="s" s="2">
-        <v>80</v>
+        <v>559</v>
       </c>
       <c r="AO83" t="s" s="2">
-        <v>80</v>
+        <v>560</v>
       </c>
     </row>
     <row r="84" hidden="true">
       <c r="A84" t="s" s="2">
-        <v>557</v>
+        <v>561</v>
       </c>
       <c r="B84" t="s" s="2">
-        <v>557</v>
+        <v>561</v>
       </c>
       <c r="C84" s="2"/>
       <c r="D84" t="s" s="2">
-        <v>558</v>
+        <v>80</v>
       </c>
       <c r="E84" s="2"/>
       <c r="F84" t="s" s="2">
@@ -11978,26 +12041,24 @@
         <v>80</v>
       </c>
       <c r="I84" t="s" s="2">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="J84" t="s" s="2">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="K84" t="s" s="2">
-        <v>138</v>
+        <v>562</v>
       </c>
       <c r="L84" t="s" s="2">
-        <v>559</v>
+        <v>563</v>
       </c>
       <c r="M84" t="s" s="2">
-        <v>560</v>
+        <v>564</v>
       </c>
       <c r="N84" t="s" s="2">
-        <v>141</v>
-      </c>
-      <c r="O84" t="s" s="2">
-        <v>175</v>
-      </c>
+        <v>565</v>
+      </c>
+      <c r="O84" s="2"/>
       <c r="P84" t="s" s="2">
         <v>80</v>
       </c>
@@ -12057,16 +12118,16 @@
         <v>102</v>
       </c>
       <c r="AJ84" t="s" s="2">
-        <v>146</v>
+        <v>103</v>
       </c>
       <c r="AK84" t="s" s="2">
-        <v>80</v>
+        <v>566</v>
       </c>
       <c r="AL84" t="s" s="2">
-        <v>80</v>
+        <v>104</v>
       </c>
       <c r="AM84" t="s" s="2">
-        <v>104</v>
+        <v>567</v>
       </c>
       <c r="AN84" t="s" s="2">
         <v>80</v>
@@ -12077,10 +12138,10 @@
     </row>
     <row r="85" hidden="true">
       <c r="A85" t="s" s="2">
-        <v>562</v>
+        <v>568</v>
       </c>
       <c r="B85" t="s" s="2">
-        <v>562</v>
+        <v>568</v>
       </c>
       <c r="C85" s="2"/>
       <c r="D85" t="s" s="2">
@@ -12088,10 +12149,10 @@
       </c>
       <c r="E85" s="2"/>
       <c r="F85" t="s" s="2">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="G85" t="s" s="2">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="H85" t="s" s="2">
         <v>80</v>
@@ -12103,17 +12164,15 @@
         <v>80</v>
       </c>
       <c r="K85" t="s" s="2">
-        <v>194</v>
+        <v>569</v>
       </c>
       <c r="L85" t="s" s="2">
-        <v>563</v>
+        <v>570</v>
       </c>
       <c r="M85" t="s" s="2">
-        <v>564</v>
-      </c>
-      <c r="N85" t="s" s="2">
-        <v>280</v>
-      </c>
+        <v>571</v>
+      </c>
+      <c r="N85" s="2"/>
       <c r="O85" s="2"/>
       <c r="P85" t="s" s="2">
         <v>80</v>
@@ -12162,13 +12221,13 @@
         <v>80</v>
       </c>
       <c r="AF85" t="s" s="2">
-        <v>562</v>
+        <v>568</v>
       </c>
       <c r="AG85" t="s" s="2">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="AH85" t="s" s="2">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="AI85" t="s" s="2">
         <v>102</v>
@@ -12177,7 +12236,7 @@
         <v>103</v>
       </c>
       <c r="AK85" t="s" s="2">
-        <v>565</v>
+        <v>572</v>
       </c>
       <c r="AL85" t="s" s="2">
         <v>80</v>
@@ -12186,7 +12245,7 @@
         <v>111</v>
       </c>
       <c r="AN85" t="s" s="2">
-        <v>566</v>
+        <v>573</v>
       </c>
       <c r="AO85" t="s" s="2">
         <v>80</v>
@@ -12194,10 +12253,10 @@
     </row>
     <row r="86" hidden="true">
       <c r="A86" t="s" s="2">
-        <v>567</v>
+        <v>574</v>
       </c>
       <c r="B86" t="s" s="2">
-        <v>567</v>
+        <v>574</v>
       </c>
       <c r="C86" s="2"/>
       <c r="D86" t="s" s="2">
@@ -12220,17 +12279,15 @@
         <v>80</v>
       </c>
       <c r="K86" t="s" s="2">
-        <v>216</v>
+        <v>194</v>
       </c>
       <c r="L86" t="s" s="2">
-        <v>568</v>
+        <v>195</v>
       </c>
       <c r="M86" t="s" s="2">
-        <v>569</v>
-      </c>
-      <c r="N86" t="s" s="2">
-        <v>310</v>
-      </c>
+        <v>196</v>
+      </c>
+      <c r="N86" s="2"/>
       <c r="O86" s="2"/>
       <c r="P86" t="s" s="2">
         <v>80</v>
@@ -12279,7 +12336,7 @@
         <v>80</v>
       </c>
       <c r="AF86" t="s" s="2">
-        <v>567</v>
+        <v>197</v>
       </c>
       <c r="AG86" t="s" s="2">
         <v>78</v>
@@ -12288,22 +12345,22 @@
         <v>90</v>
       </c>
       <c r="AI86" t="s" s="2">
-        <v>102</v>
+        <v>80</v>
       </c>
       <c r="AJ86" t="s" s="2">
-        <v>103</v>
+        <v>80</v>
       </c>
       <c r="AK86" t="s" s="2">
-        <v>570</v>
+        <v>80</v>
       </c>
       <c r="AL86" t="s" s="2">
-        <v>314</v>
+        <v>80</v>
       </c>
       <c r="AM86" t="s" s="2">
-        <v>315</v>
+        <v>111</v>
       </c>
       <c r="AN86" t="s" s="2">
-        <v>571</v>
+        <v>80</v>
       </c>
       <c r="AO86" t="s" s="2">
         <v>80</v>
@@ -12311,21 +12368,21 @@
     </row>
     <row r="87" hidden="true">
       <c r="A87" t="s" s="2">
-        <v>572</v>
+        <v>575</v>
       </c>
       <c r="B87" t="s" s="2">
-        <v>572</v>
+        <v>575</v>
       </c>
       <c r="C87" s="2"/>
       <c r="D87" t="s" s="2">
-        <v>80</v>
+        <v>137</v>
       </c>
       <c r="E87" s="2"/>
       <c r="F87" t="s" s="2">
         <v>78</v>
       </c>
       <c r="G87" t="s" s="2">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="H87" t="s" s="2">
         <v>80</v>
@@ -12337,16 +12394,16 @@
         <v>80</v>
       </c>
       <c r="K87" t="s" s="2">
-        <v>194</v>
+        <v>138</v>
       </c>
       <c r="L87" t="s" s="2">
-        <v>573</v>
+        <v>139</v>
       </c>
       <c r="M87" t="s" s="2">
-        <v>574</v>
+        <v>200</v>
       </c>
       <c r="N87" t="s" s="2">
-        <v>280</v>
+        <v>141</v>
       </c>
       <c r="O87" s="2"/>
       <c r="P87" t="s" s="2">
@@ -12384,43 +12441,43 @@
         <v>80</v>
       </c>
       <c r="AB87" t="s" s="2">
-        <v>80</v>
+        <v>142</v>
       </c>
       <c r="AC87" t="s" s="2">
-        <v>80</v>
+        <v>143</v>
       </c>
       <c r="AD87" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AE87" t="s" s="2">
-        <v>80</v>
+        <v>144</v>
       </c>
       <c r="AF87" t="s" s="2">
-        <v>572</v>
+        <v>201</v>
       </c>
       <c r="AG87" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AH87" t="s" s="2">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="AI87" t="s" s="2">
         <v>102</v>
       </c>
       <c r="AJ87" t="s" s="2">
-        <v>103</v>
+        <v>146</v>
       </c>
       <c r="AK87" t="s" s="2">
-        <v>575</v>
+        <v>80</v>
       </c>
       <c r="AL87" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AM87" t="s" s="2">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="AN87" t="s" s="2">
-        <v>576</v>
+        <v>80</v>
       </c>
       <c r="AO87" t="s" s="2">
         <v>80</v>
@@ -12428,14 +12485,14 @@
     </row>
     <row r="88" hidden="true">
       <c r="A88" t="s" s="2">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B88" t="s" s="2">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="C88" s="2"/>
       <c r="D88" t="s" s="2">
-        <v>80</v>
+        <v>577</v>
       </c>
       <c r="E88" s="2"/>
       <c r="F88" t="s" s="2">
@@ -12448,13 +12505,13 @@
         <v>80</v>
       </c>
       <c r="I88" t="s" s="2">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="J88" t="s" s="2">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="K88" t="s" s="2">
-        <v>550</v>
+        <v>138</v>
       </c>
       <c r="L88" t="s" s="2">
         <v>578</v>
@@ -12462,8 +12519,12 @@
       <c r="M88" t="s" s="2">
         <v>579</v>
       </c>
-      <c r="N88" s="2"/>
-      <c r="O88" s="2"/>
+      <c r="N88" t="s" s="2">
+        <v>141</v>
+      </c>
+      <c r="O88" t="s" s="2">
+        <v>175</v>
+      </c>
       <c r="P88" t="s" s="2">
         <v>80</v>
       </c>
@@ -12511,7 +12572,7 @@
         <v>80</v>
       </c>
       <c r="AF88" t="s" s="2">
-        <v>577</v>
+        <v>580</v>
       </c>
       <c r="AG88" t="s" s="2">
         <v>78</v>
@@ -12523,16 +12584,16 @@
         <v>102</v>
       </c>
       <c r="AJ88" t="s" s="2">
-        <v>103</v>
+        <v>146</v>
       </c>
       <c r="AK88" t="s" s="2">
-        <v>580</v>
+        <v>80</v>
       </c>
       <c r="AL88" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AM88" t="s" s="2">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="AN88" t="s" s="2">
         <v>80</v>
@@ -12554,7 +12615,7 @@
       </c>
       <c r="E89" s="2"/>
       <c r="F89" t="s" s="2">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="G89" t="s" s="2">
         <v>90</v>
@@ -12572,12 +12633,14 @@
         <v>194</v>
       </c>
       <c r="L89" t="s" s="2">
-        <v>195</v>
+        <v>582</v>
       </c>
       <c r="M89" t="s" s="2">
-        <v>196</v>
-      </c>
-      <c r="N89" s="2"/>
+        <v>583</v>
+      </c>
+      <c r="N89" t="s" s="2">
+        <v>280</v>
+      </c>
       <c r="O89" s="2"/>
       <c r="P89" t="s" s="2">
         <v>80</v>
@@ -12626,22 +12689,22 @@
         <v>80</v>
       </c>
       <c r="AF89" t="s" s="2">
-        <v>197</v>
+        <v>581</v>
       </c>
       <c r="AG89" t="s" s="2">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="AH89" t="s" s="2">
         <v>90</v>
       </c>
       <c r="AI89" t="s" s="2">
-        <v>80</v>
+        <v>102</v>
       </c>
       <c r="AJ89" t="s" s="2">
-        <v>80</v>
+        <v>103</v>
       </c>
       <c r="AK89" t="s" s="2">
-        <v>80</v>
+        <v>584</v>
       </c>
       <c r="AL89" t="s" s="2">
         <v>80</v>
@@ -12650,7 +12713,7 @@
         <v>111</v>
       </c>
       <c r="AN89" t="s" s="2">
-        <v>80</v>
+        <v>585</v>
       </c>
       <c r="AO89" t="s" s="2">
         <v>80</v>
@@ -12658,21 +12721,21 @@
     </row>
     <row r="90" hidden="true">
       <c r="A90" t="s" s="2">
-        <v>582</v>
+        <v>586</v>
       </c>
       <c r="B90" t="s" s="2">
-        <v>582</v>
+        <v>586</v>
       </c>
       <c r="C90" s="2"/>
       <c r="D90" t="s" s="2">
-        <v>137</v>
+        <v>80</v>
       </c>
       <c r="E90" s="2"/>
       <c r="F90" t="s" s="2">
         <v>78</v>
       </c>
       <c r="G90" t="s" s="2">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="H90" t="s" s="2">
         <v>80</v>
@@ -12684,16 +12747,16 @@
         <v>80</v>
       </c>
       <c r="K90" t="s" s="2">
-        <v>138</v>
+        <v>216</v>
       </c>
       <c r="L90" t="s" s="2">
-        <v>139</v>
+        <v>587</v>
       </c>
       <c r="M90" t="s" s="2">
-        <v>200</v>
+        <v>588</v>
       </c>
       <c r="N90" t="s" s="2">
-        <v>141</v>
+        <v>310</v>
       </c>
       <c r="O90" s="2"/>
       <c r="P90" t="s" s="2">
@@ -12731,43 +12794,43 @@
         <v>80</v>
       </c>
       <c r="AB90" t="s" s="2">
-        <v>142</v>
+        <v>80</v>
       </c>
       <c r="AC90" t="s" s="2">
-        <v>143</v>
+        <v>80</v>
       </c>
       <c r="AD90" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AE90" t="s" s="2">
-        <v>144</v>
+        <v>80</v>
       </c>
       <c r="AF90" t="s" s="2">
-        <v>201</v>
+        <v>586</v>
       </c>
       <c r="AG90" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AH90" t="s" s="2">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="AI90" t="s" s="2">
         <v>102</v>
       </c>
       <c r="AJ90" t="s" s="2">
-        <v>146</v>
+        <v>103</v>
       </c>
       <c r="AK90" t="s" s="2">
-        <v>80</v>
+        <v>589</v>
       </c>
       <c r="AL90" t="s" s="2">
-        <v>80</v>
+        <v>314</v>
       </c>
       <c r="AM90" t="s" s="2">
-        <v>104</v>
+        <v>315</v>
       </c>
       <c r="AN90" t="s" s="2">
-        <v>80</v>
+        <v>590</v>
       </c>
       <c r="AO90" t="s" s="2">
         <v>80</v>
@@ -12775,46 +12838,44 @@
     </row>
     <row r="91" hidden="true">
       <c r="A91" t="s" s="2">
-        <v>583</v>
+        <v>591</v>
       </c>
       <c r="B91" t="s" s="2">
-        <v>583</v>
+        <v>591</v>
       </c>
       <c r="C91" s="2"/>
       <c r="D91" t="s" s="2">
-        <v>558</v>
+        <v>80</v>
       </c>
       <c r="E91" s="2"/>
       <c r="F91" t="s" s="2">
         <v>78</v>
       </c>
       <c r="G91" t="s" s="2">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="H91" t="s" s="2">
         <v>80</v>
       </c>
       <c r="I91" t="s" s="2">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="J91" t="s" s="2">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="K91" t="s" s="2">
-        <v>138</v>
+        <v>194</v>
       </c>
       <c r="L91" t="s" s="2">
-        <v>559</v>
+        <v>592</v>
       </c>
       <c r="M91" t="s" s="2">
-        <v>560</v>
+        <v>593</v>
       </c>
       <c r="N91" t="s" s="2">
-        <v>141</v>
-      </c>
-      <c r="O91" t="s" s="2">
-        <v>175</v>
-      </c>
+        <v>280</v>
+      </c>
+      <c r="O91" s="2"/>
       <c r="P91" t="s" s="2">
         <v>80</v>
       </c>
@@ -12862,31 +12923,31 @@
         <v>80</v>
       </c>
       <c r="AF91" t="s" s="2">
-        <v>561</v>
+        <v>591</v>
       </c>
       <c r="AG91" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AH91" t="s" s="2">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="AI91" t="s" s="2">
         <v>102</v>
       </c>
       <c r="AJ91" t="s" s="2">
-        <v>146</v>
+        <v>103</v>
       </c>
       <c r="AK91" t="s" s="2">
-        <v>80</v>
+        <v>594</v>
       </c>
       <c r="AL91" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AM91" t="s" s="2">
-        <v>104</v>
+        <v>111</v>
       </c>
       <c r="AN91" t="s" s="2">
-        <v>80</v>
+        <v>595</v>
       </c>
       <c r="AO91" t="s" s="2">
         <v>80</v>
@@ -12894,10 +12955,10 @@
     </row>
     <row r="92" hidden="true">
       <c r="A92" t="s" s="2">
-        <v>584</v>
+        <v>596</v>
       </c>
       <c r="B92" t="s" s="2">
-        <v>584</v>
+        <v>596</v>
       </c>
       <c r="C92" s="2"/>
       <c r="D92" t="s" s="2">
@@ -12908,7 +12969,7 @@
         <v>78</v>
       </c>
       <c r="G92" t="s" s="2">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="H92" t="s" s="2">
         <v>80</v>
@@ -12920,17 +12981,15 @@
         <v>80</v>
       </c>
       <c r="K92" t="s" s="2">
-        <v>194</v>
+        <v>569</v>
       </c>
       <c r="L92" t="s" s="2">
-        <v>585</v>
+        <v>597</v>
       </c>
       <c r="M92" t="s" s="2">
-        <v>586</v>
-      </c>
-      <c r="N92" t="s" s="2">
-        <v>280</v>
-      </c>
+        <v>598</v>
+      </c>
+      <c r="N92" s="2"/>
       <c r="O92" s="2"/>
       <c r="P92" t="s" s="2">
         <v>80</v>
@@ -12979,13 +13038,13 @@
         <v>80</v>
       </c>
       <c r="AF92" t="s" s="2">
-        <v>584</v>
+        <v>596</v>
       </c>
       <c r="AG92" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AH92" t="s" s="2">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="AI92" t="s" s="2">
         <v>102</v>
@@ -12994,7 +13053,7 @@
         <v>103</v>
       </c>
       <c r="AK92" t="s" s="2">
-        <v>587</v>
+        <v>599</v>
       </c>
       <c r="AL92" t="s" s="2">
         <v>80</v>
@@ -13011,10 +13070,10 @@
     </row>
     <row r="93" hidden="true">
       <c r="A93" t="s" s="2">
-        <v>588</v>
+        <v>600</v>
       </c>
       <c r="B93" t="s" s="2">
-        <v>588</v>
+        <v>600</v>
       </c>
       <c r="C93" s="2"/>
       <c r="D93" t="s" s="2">
@@ -13037,17 +13096,15 @@
         <v>80</v>
       </c>
       <c r="K93" t="s" s="2">
-        <v>216</v>
+        <v>194</v>
       </c>
       <c r="L93" t="s" s="2">
-        <v>589</v>
+        <v>195</v>
       </c>
       <c r="M93" t="s" s="2">
-        <v>590</v>
-      </c>
-      <c r="N93" t="s" s="2">
-        <v>310</v>
-      </c>
+        <v>196</v>
+      </c>
+      <c r="N93" s="2"/>
       <c r="O93" s="2"/>
       <c r="P93" t="s" s="2">
         <v>80</v>
@@ -13072,13 +13129,13 @@
         <v>80</v>
       </c>
       <c r="X93" t="s" s="2">
-        <v>117</v>
+        <v>80</v>
       </c>
       <c r="Y93" t="s" s="2">
-        <v>591</v>
+        <v>80</v>
       </c>
       <c r="Z93" t="s" s="2">
-        <v>592</v>
+        <v>80</v>
       </c>
       <c r="AA93" t="s" s="2">
         <v>80</v>
@@ -13096,7 +13153,7 @@
         <v>80</v>
       </c>
       <c r="AF93" t="s" s="2">
-        <v>588</v>
+        <v>197</v>
       </c>
       <c r="AG93" t="s" s="2">
         <v>78</v>
@@ -13105,29 +13162,499 @@
         <v>90</v>
       </c>
       <c r="AI93" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AJ93" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AK93" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AL93" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AM93" t="s" s="2">
+        <v>111</v>
+      </c>
+      <c r="AN93" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AO93" t="s" s="2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="94" hidden="true">
+      <c r="A94" t="s" s="2">
+        <v>601</v>
+      </c>
+      <c r="B94" t="s" s="2">
+        <v>601</v>
+      </c>
+      <c r="C94" s="2"/>
+      <c r="D94" t="s" s="2">
+        <v>137</v>
+      </c>
+      <c r="E94" s="2"/>
+      <c r="F94" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="G94" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="H94" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="I94" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="J94" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="K94" t="s" s="2">
+        <v>138</v>
+      </c>
+      <c r="L94" t="s" s="2">
+        <v>139</v>
+      </c>
+      <c r="M94" t="s" s="2">
+        <v>200</v>
+      </c>
+      <c r="N94" t="s" s="2">
+        <v>141</v>
+      </c>
+      <c r="O94" s="2"/>
+      <c r="P94" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="Q94" s="2"/>
+      <c r="R94" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="S94" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="T94" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="U94" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="V94" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="W94" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="X94" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="Y94" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="Z94" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AA94" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AB94" t="s" s="2">
+        <v>142</v>
+      </c>
+      <c r="AC94" t="s" s="2">
+        <v>143</v>
+      </c>
+      <c r="AD94" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AE94" t="s" s="2">
+        <v>144</v>
+      </c>
+      <c r="AF94" t="s" s="2">
+        <v>201</v>
+      </c>
+      <c r="AG94" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AH94" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AI94" t="s" s="2">
         <v>102</v>
       </c>
-      <c r="AJ93" t="s" s="2">
+      <c r="AJ94" t="s" s="2">
+        <v>146</v>
+      </c>
+      <c r="AK94" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AL94" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AM94" t="s" s="2">
+        <v>104</v>
+      </c>
+      <c r="AN94" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AO94" t="s" s="2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="95" hidden="true">
+      <c r="A95" t="s" s="2">
+        <v>602</v>
+      </c>
+      <c r="B95" t="s" s="2">
+        <v>602</v>
+      </c>
+      <c r="C95" s="2"/>
+      <c r="D95" t="s" s="2">
+        <v>577</v>
+      </c>
+      <c r="E95" s="2"/>
+      <c r="F95" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="G95" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="H95" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="I95" t="s" s="2">
+        <v>91</v>
+      </c>
+      <c r="J95" t="s" s="2">
+        <v>91</v>
+      </c>
+      <c r="K95" t="s" s="2">
+        <v>138</v>
+      </c>
+      <c r="L95" t="s" s="2">
+        <v>578</v>
+      </c>
+      <c r="M95" t="s" s="2">
+        <v>579</v>
+      </c>
+      <c r="N95" t="s" s="2">
+        <v>141</v>
+      </c>
+      <c r="O95" t="s" s="2">
+        <v>175</v>
+      </c>
+      <c r="P95" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="Q95" s="2"/>
+      <c r="R95" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="S95" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="T95" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="U95" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="V95" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="W95" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="X95" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="Y95" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="Z95" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AA95" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AB95" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AC95" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AD95" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AE95" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AF95" t="s" s="2">
+        <v>580</v>
+      </c>
+      <c r="AG95" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AH95" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AI95" t="s" s="2">
+        <v>102</v>
+      </c>
+      <c r="AJ95" t="s" s="2">
+        <v>146</v>
+      </c>
+      <c r="AK95" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AL95" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AM95" t="s" s="2">
+        <v>104</v>
+      </c>
+      <c r="AN95" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AO95" t="s" s="2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="96" hidden="true">
+      <c r="A96" t="s" s="2">
+        <v>603</v>
+      </c>
+      <c r="B96" t="s" s="2">
+        <v>603</v>
+      </c>
+      <c r="C96" s="2"/>
+      <c r="D96" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="E96" s="2"/>
+      <c r="F96" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="G96" t="s" s="2">
+        <v>90</v>
+      </c>
+      <c r="H96" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="I96" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="J96" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="K96" t="s" s="2">
+        <v>194</v>
+      </c>
+      <c r="L96" t="s" s="2">
+        <v>604</v>
+      </c>
+      <c r="M96" t="s" s="2">
+        <v>605</v>
+      </c>
+      <c r="N96" t="s" s="2">
+        <v>280</v>
+      </c>
+      <c r="O96" s="2"/>
+      <c r="P96" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="Q96" s="2"/>
+      <c r="R96" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="S96" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="T96" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="U96" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="V96" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="W96" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="X96" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="Y96" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="Z96" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AA96" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AB96" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AC96" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AD96" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AE96" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AF96" t="s" s="2">
+        <v>603</v>
+      </c>
+      <c r="AG96" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AH96" t="s" s="2">
+        <v>90</v>
+      </c>
+      <c r="AI96" t="s" s="2">
+        <v>102</v>
+      </c>
+      <c r="AJ96" t="s" s="2">
         <v>103</v>
       </c>
-      <c r="AK93" t="s" s="2">
-        <v>593</v>
-      </c>
-      <c r="AL93" t="s" s="2">
+      <c r="AK96" t="s" s="2">
+        <v>606</v>
+      </c>
+      <c r="AL96" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AM96" t="s" s="2">
+        <v>111</v>
+      </c>
+      <c r="AN96" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AO96" t="s" s="2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="97" hidden="true">
+      <c r="A97" t="s" s="2">
+        <v>607</v>
+      </c>
+      <c r="B97" t="s" s="2">
+        <v>607</v>
+      </c>
+      <c r="C97" s="2"/>
+      <c r="D97" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="E97" s="2"/>
+      <c r="F97" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="G97" t="s" s="2">
+        <v>90</v>
+      </c>
+      <c r="H97" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="I97" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="J97" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="K97" t="s" s="2">
+        <v>216</v>
+      </c>
+      <c r="L97" t="s" s="2">
+        <v>608</v>
+      </c>
+      <c r="M97" t="s" s="2">
+        <v>609</v>
+      </c>
+      <c r="N97" t="s" s="2">
+        <v>310</v>
+      </c>
+      <c r="O97" s="2"/>
+      <c r="P97" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="Q97" s="2"/>
+      <c r="R97" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="S97" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="T97" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="U97" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="V97" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="W97" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="X97" t="s" s="2">
+        <v>117</v>
+      </c>
+      <c r="Y97" t="s" s="2">
+        <v>610</v>
+      </c>
+      <c r="Z97" t="s" s="2">
+        <v>611</v>
+      </c>
+      <c r="AA97" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AB97" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AC97" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AD97" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AE97" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AF97" t="s" s="2">
+        <v>607</v>
+      </c>
+      <c r="AG97" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AH97" t="s" s="2">
+        <v>90</v>
+      </c>
+      <c r="AI97" t="s" s="2">
+        <v>102</v>
+      </c>
+      <c r="AJ97" t="s" s="2">
+        <v>103</v>
+      </c>
+      <c r="AK97" t="s" s="2">
+        <v>612</v>
+      </c>
+      <c r="AL97" t="s" s="2">
         <v>314</v>
       </c>
-      <c r="AM93" t="s" s="2">
+      <c r="AM97" t="s" s="2">
         <v>315</v>
       </c>
-      <c r="AN93" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="AO93" t="s" s="2">
+      <c r="AN97" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AO97" t="s" s="2">
         <v>80</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AO93">
+  <autoFilter ref="A1:AO97">
     <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -13137,7 +13664,7 @@
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>
-  <conditionalFormatting sqref="A2:AI92">
+  <conditionalFormatting sqref="A2:AI96">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$G2&lt;&gt;"Y"</formula>
     </cfRule>

</xml_diff>

<commit_message>
modif short description (#124) 3df06a79116b7705f86f9e7f3b8a5226a5bab5c9
</commit_message>
<xml_diff>
--- a/ig/main/StructureDefinition-eclaire-researchstudy.xlsx
+++ b/ig/main/StructureDefinition-eclaire-researchstudy.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-02-15T13:54:33+00:00</t>
+    <t>2024-02-15T16:42:49+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -1690,7 +1690,7 @@
     <t>ResearchStudy.description</t>
   </si>
   <si>
-    <t>Résumé de l'essai / Summary Results</t>
+    <t>Résumé de l'essai (description, durée de participation à l'essai clinique,etc) / Summary Results</t>
   </si>
   <si>
     <t>A full description of how the study is being conducted.</t>

</xml_diff>

<commit_message>
add short primary purpose (#126)
* add short primary purpose

* Maj mapping primaryPurposeType

---------

Co-authored-by: sly-kereval <125375447+sly-kereval@users.noreply.github.com> d79356d36c77b4ececf492fff16d45cdce818216
</commit_message>
<xml_diff>
--- a/ig/main/StructureDefinition-eclaire-researchstudy.xlsx
+++ b/ig/main/StructureDefinition-eclaire-researchstudy.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-02-15T16:43:54+00:00</t>
+    <t>2024-02-15T17:28:18+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -1155,7 +1155,7 @@
     <t>ResearchStudy.primaryPurposeType</t>
   </si>
   <si>
-    <t>treatment | prevention | diagnostic | supportive-care | screening | health-services-research | basic-science | device-feasibility</t>
+    <t>Objectif principal / Primary purpose</t>
   </si>
   <si>
     <t>The type of study based upon the intent of the study's activities. A classification of the intent of the study.</t>
@@ -8182,7 +8182,7 @@
         <v>90</v>
       </c>
       <c r="H50" t="s" s="2">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="I50" t="s" s="2">
         <v>80</v>

</xml_diff>

<commit_message>
add extension ECLAIREArmIntervention (#127)
* add extension ECLAIREArmIntervention

* Maj mapping intervention

---------

Co-authored-by: sly-kereval <125375447+sly-kereval@users.noreply.github.com> 768e8280ae2c18b9f89ec8f64d21cc800fa17bbb
</commit_message>
<xml_diff>
--- a/ig/main/StructureDefinition-eclaire-researchstudy.xlsx
+++ b/ig/main/StructureDefinition-eclaire-researchstudy.xlsx
@@ -10,13 +10,13 @@
     <sheet name="Elements" r:id="rId4" sheetId="2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="true">Elements!$A$1:$AO$108</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="true">Elements!$A$1:$AO$109</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4040" uniqueCount="656">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4077" uniqueCount="661">
   <si>
     <t>Property</t>
   </si>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-02-15T17:28:18+00:00</t>
+    <t>2024-02-16T08:51:01+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -1933,6 +1933,22 @@
   </si>
   <si>
     <t>ResearchStudy.arm.extension</t>
+  </si>
+  <si>
+    <t>ResearchStudy.arm.extension:eclaire-arm-intervention</t>
+  </si>
+  <si>
+    <t>eclaire-arm-intervention</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extension {https://interop.esante.gouv.fr/ig/fhir/eclaire/StructureDefinition/eclaire-arm-intervention}
+</t>
+  </si>
+  <si>
+    <t>Intervention / For each arm of the trial record a brief intervention name plus an intervention description.</t>
+  </si>
+  <si>
+    <t>Extension créée dans le cadre du projet ECLAIRE pour indiquer les 'Interventions' dans les cohortes</t>
   </si>
   <si>
     <t>ResearchStudy.arm.modifierExtension</t>
@@ -2363,7 +2379,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AO108"/>
+  <dimension ref="A1:AO109"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -13901,11 +13917,13 @@
         <v>619</v>
       </c>
       <c r="B99" t="s" s="2">
-        <v>619</v>
-      </c>
-      <c r="C99" s="2"/>
+        <v>618</v>
+      </c>
+      <c r="C99" t="s" s="2">
+        <v>620</v>
+      </c>
       <c r="D99" t="s" s="2">
-        <v>620</v>
+        <v>80</v>
       </c>
       <c r="E99" s="2"/>
       <c r="F99" t="s" s="2">
@@ -13915,29 +13933,25 @@
         <v>79</v>
       </c>
       <c r="H99" t="s" s="2">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="I99" t="s" s="2">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="J99" t="s" s="2">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="K99" t="s" s="2">
-        <v>138</v>
+        <v>621</v>
       </c>
       <c r="L99" t="s" s="2">
-        <v>621</v>
+        <v>622</v>
       </c>
       <c r="M99" t="s" s="2">
-        <v>622</v>
-      </c>
-      <c r="N99" t="s" s="2">
-        <v>141</v>
-      </c>
-      <c r="O99" t="s" s="2">
-        <v>214</v>
-      </c>
+        <v>623</v>
+      </c>
+      <c r="N99" s="2"/>
+      <c r="O99" s="2"/>
       <c r="P99" t="s" s="2">
         <v>80</v>
       </c>
@@ -13985,7 +13999,7 @@
         <v>80</v>
       </c>
       <c r="AF99" t="s" s="2">
-        <v>623</v>
+        <v>187</v>
       </c>
       <c r="AG99" t="s" s="2">
         <v>78</v>
@@ -14006,7 +14020,7 @@
         <v>80</v>
       </c>
       <c r="AM99" t="s" s="2">
-        <v>104</v>
+        <v>80</v>
       </c>
       <c r="AN99" t="s" s="2">
         <v>80</v>
@@ -14024,37 +14038,39 @@
       </c>
       <c r="C100" s="2"/>
       <c r="D100" t="s" s="2">
-        <v>80</v>
+        <v>625</v>
       </c>
       <c r="E100" s="2"/>
       <c r="F100" t="s" s="2">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="G100" t="s" s="2">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="H100" t="s" s="2">
         <v>80</v>
       </c>
       <c r="I100" t="s" s="2">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="J100" t="s" s="2">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="K100" t="s" s="2">
-        <v>179</v>
+        <v>138</v>
       </c>
       <c r="L100" t="s" s="2">
-        <v>625</v>
+        <v>626</v>
       </c>
       <c r="M100" t="s" s="2">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="N100" t="s" s="2">
-        <v>337</v>
-      </c>
-      <c r="O100" s="2"/>
+        <v>141</v>
+      </c>
+      <c r="O100" t="s" s="2">
+        <v>214</v>
+      </c>
       <c r="P100" t="s" s="2">
         <v>80</v>
       </c>
@@ -14102,31 +14118,31 @@
         <v>80</v>
       </c>
       <c r="AF100" t="s" s="2">
-        <v>624</v>
+        <v>628</v>
       </c>
       <c r="AG100" t="s" s="2">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="AH100" t="s" s="2">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="AI100" t="s" s="2">
         <v>102</v>
       </c>
       <c r="AJ100" t="s" s="2">
-        <v>103</v>
+        <v>146</v>
       </c>
       <c r="AK100" t="s" s="2">
-        <v>627</v>
+        <v>80</v>
       </c>
       <c r="AL100" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AM100" t="s" s="2">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="AN100" t="s" s="2">
-        <v>628</v>
+        <v>80</v>
       </c>
       <c r="AO100" t="s" s="2">
         <v>80</v>
@@ -14145,7 +14161,7 @@
       </c>
       <c r="E101" s="2"/>
       <c r="F101" t="s" s="2">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="G101" t="s" s="2">
         <v>90</v>
@@ -14160,7 +14176,7 @@
         <v>80</v>
       </c>
       <c r="K101" t="s" s="2">
-        <v>250</v>
+        <v>179</v>
       </c>
       <c r="L101" t="s" s="2">
         <v>630</v>
@@ -14169,7 +14185,7 @@
         <v>631</v>
       </c>
       <c r="N101" t="s" s="2">
-        <v>367</v>
+        <v>337</v>
       </c>
       <c r="O101" s="2"/>
       <c r="P101" t="s" s="2">
@@ -14222,7 +14238,7 @@
         <v>629</v>
       </c>
       <c r="AG101" t="s" s="2">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="AH101" t="s" s="2">
         <v>90</v>
@@ -14237,10 +14253,10 @@
         <v>632</v>
       </c>
       <c r="AL101" t="s" s="2">
-        <v>371</v>
+        <v>80</v>
       </c>
       <c r="AM101" t="s" s="2">
-        <v>372</v>
+        <v>111</v>
       </c>
       <c r="AN101" t="s" s="2">
         <v>633</v>
@@ -14277,7 +14293,7 @@
         <v>80</v>
       </c>
       <c r="K102" t="s" s="2">
-        <v>179</v>
+        <v>250</v>
       </c>
       <c r="L102" t="s" s="2">
         <v>635</v>
@@ -14286,7 +14302,7 @@
         <v>636</v>
       </c>
       <c r="N102" t="s" s="2">
-        <v>337</v>
+        <v>367</v>
       </c>
       <c r="O102" s="2"/>
       <c r="P102" t="s" s="2">
@@ -14354,10 +14370,10 @@
         <v>637</v>
       </c>
       <c r="AL102" t="s" s="2">
-        <v>80</v>
+        <v>371</v>
       </c>
       <c r="AM102" t="s" s="2">
-        <v>111</v>
+        <v>372</v>
       </c>
       <c r="AN102" t="s" s="2">
         <v>638</v>
@@ -14382,7 +14398,7 @@
         <v>78</v>
       </c>
       <c r="G103" t="s" s="2">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="H103" t="s" s="2">
         <v>80</v>
@@ -14394,7 +14410,7 @@
         <v>80</v>
       </c>
       <c r="K103" t="s" s="2">
-        <v>612</v>
+        <v>179</v>
       </c>
       <c r="L103" t="s" s="2">
         <v>640</v>
@@ -14402,7 +14418,9 @@
       <c r="M103" t="s" s="2">
         <v>641</v>
       </c>
-      <c r="N103" s="2"/>
+      <c r="N103" t="s" s="2">
+        <v>337</v>
+      </c>
       <c r="O103" s="2"/>
       <c r="P103" t="s" s="2">
         <v>80</v>
@@ -14457,7 +14475,7 @@
         <v>78</v>
       </c>
       <c r="AH103" t="s" s="2">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="AI103" t="s" s="2">
         <v>102</v>
@@ -14475,7 +14493,7 @@
         <v>111</v>
       </c>
       <c r="AN103" t="s" s="2">
-        <v>80</v>
+        <v>643</v>
       </c>
       <c r="AO103" t="s" s="2">
         <v>80</v>
@@ -14483,10 +14501,10 @@
     </row>
     <row r="104" hidden="true">
       <c r="A104" t="s" s="2">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="B104" t="s" s="2">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="C104" s="2"/>
       <c r="D104" t="s" s="2">
@@ -14497,7 +14515,7 @@
         <v>78</v>
       </c>
       <c r="G104" t="s" s="2">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="H104" t="s" s="2">
         <v>80</v>
@@ -14509,13 +14527,13 @@
         <v>80</v>
       </c>
       <c r="K104" t="s" s="2">
-        <v>179</v>
+        <v>612</v>
       </c>
       <c r="L104" t="s" s="2">
-        <v>180</v>
+        <v>645</v>
       </c>
       <c r="M104" t="s" s="2">
-        <v>181</v>
+        <v>646</v>
       </c>
       <c r="N104" s="2"/>
       <c r="O104" s="2"/>
@@ -14566,22 +14584,22 @@
         <v>80</v>
       </c>
       <c r="AF104" t="s" s="2">
-        <v>182</v>
+        <v>644</v>
       </c>
       <c r="AG104" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AH104" t="s" s="2">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="AI104" t="s" s="2">
-        <v>80</v>
+        <v>102</v>
       </c>
       <c r="AJ104" t="s" s="2">
-        <v>80</v>
+        <v>103</v>
       </c>
       <c r="AK104" t="s" s="2">
-        <v>80</v>
+        <v>647</v>
       </c>
       <c r="AL104" t="s" s="2">
         <v>80</v>
@@ -14598,21 +14616,21 @@
     </row>
     <row r="105" hidden="true">
       <c r="A105" t="s" s="2">
-        <v>644</v>
+        <v>648</v>
       </c>
       <c r="B105" t="s" s="2">
-        <v>644</v>
+        <v>648</v>
       </c>
       <c r="C105" s="2"/>
       <c r="D105" t="s" s="2">
-        <v>137</v>
+        <v>80</v>
       </c>
       <c r="E105" s="2"/>
       <c r="F105" t="s" s="2">
         <v>78</v>
       </c>
       <c r="G105" t="s" s="2">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="H105" t="s" s="2">
         <v>80</v>
@@ -14624,17 +14642,15 @@
         <v>80</v>
       </c>
       <c r="K105" t="s" s="2">
-        <v>138</v>
+        <v>179</v>
       </c>
       <c r="L105" t="s" s="2">
-        <v>139</v>
+        <v>180</v>
       </c>
       <c r="M105" t="s" s="2">
-        <v>235</v>
-      </c>
-      <c r="N105" t="s" s="2">
-        <v>141</v>
-      </c>
+        <v>181</v>
+      </c>
+      <c r="N105" s="2"/>
       <c r="O105" s="2"/>
       <c r="P105" t="s" s="2">
         <v>80</v>
@@ -14671,31 +14687,31 @@
         <v>80</v>
       </c>
       <c r="AB105" t="s" s="2">
-        <v>142</v>
+        <v>80</v>
       </c>
       <c r="AC105" t="s" s="2">
-        <v>143</v>
+        <v>80</v>
       </c>
       <c r="AD105" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AE105" t="s" s="2">
-        <v>144</v>
+        <v>80</v>
       </c>
       <c r="AF105" t="s" s="2">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="AG105" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AH105" t="s" s="2">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="AI105" t="s" s="2">
-        <v>102</v>
+        <v>80</v>
       </c>
       <c r="AJ105" t="s" s="2">
-        <v>146</v>
+        <v>80</v>
       </c>
       <c r="AK105" t="s" s="2">
         <v>80</v>
@@ -14704,7 +14720,7 @@
         <v>80</v>
       </c>
       <c r="AM105" t="s" s="2">
-        <v>104</v>
+        <v>111</v>
       </c>
       <c r="AN105" t="s" s="2">
         <v>80</v>
@@ -14715,14 +14731,14 @@
     </row>
     <row r="106" hidden="true">
       <c r="A106" t="s" s="2">
-        <v>645</v>
+        <v>649</v>
       </c>
       <c r="B106" t="s" s="2">
-        <v>645</v>
+        <v>649</v>
       </c>
       <c r="C106" s="2"/>
       <c r="D106" t="s" s="2">
-        <v>620</v>
+        <v>137</v>
       </c>
       <c r="E106" s="2"/>
       <c r="F106" t="s" s="2">
@@ -14735,26 +14751,24 @@
         <v>80</v>
       </c>
       <c r="I106" t="s" s="2">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="J106" t="s" s="2">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="K106" t="s" s="2">
         <v>138</v>
       </c>
       <c r="L106" t="s" s="2">
-        <v>621</v>
+        <v>139</v>
       </c>
       <c r="M106" t="s" s="2">
-        <v>622</v>
+        <v>235</v>
       </c>
       <c r="N106" t="s" s="2">
         <v>141</v>
       </c>
-      <c r="O106" t="s" s="2">
-        <v>214</v>
-      </c>
+      <c r="O106" s="2"/>
       <c r="P106" t="s" s="2">
         <v>80</v>
       </c>
@@ -14790,19 +14804,19 @@
         <v>80</v>
       </c>
       <c r="AB106" t="s" s="2">
-        <v>80</v>
+        <v>142</v>
       </c>
       <c r="AC106" t="s" s="2">
-        <v>80</v>
+        <v>143</v>
       </c>
       <c r="AD106" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AE106" t="s" s="2">
-        <v>80</v>
+        <v>144</v>
       </c>
       <c r="AF106" t="s" s="2">
-        <v>623</v>
+        <v>187</v>
       </c>
       <c r="AG106" t="s" s="2">
         <v>78</v>
@@ -14834,44 +14848,46 @@
     </row>
     <row r="107" hidden="true">
       <c r="A107" t="s" s="2">
-        <v>646</v>
+        <v>650</v>
       </c>
       <c r="B107" t="s" s="2">
-        <v>646</v>
+        <v>650</v>
       </c>
       <c r="C107" s="2"/>
       <c r="D107" t="s" s="2">
-        <v>80</v>
+        <v>625</v>
       </c>
       <c r="E107" s="2"/>
       <c r="F107" t="s" s="2">
         <v>78</v>
       </c>
       <c r="G107" t="s" s="2">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="H107" t="s" s="2">
         <v>80</v>
       </c>
       <c r="I107" t="s" s="2">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="J107" t="s" s="2">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="K107" t="s" s="2">
-        <v>179</v>
+        <v>138</v>
       </c>
       <c r="L107" t="s" s="2">
-        <v>647</v>
+        <v>626</v>
       </c>
       <c r="M107" t="s" s="2">
-        <v>648</v>
+        <v>627</v>
       </c>
       <c r="N107" t="s" s="2">
-        <v>337</v>
-      </c>
-      <c r="O107" s="2"/>
+        <v>141</v>
+      </c>
+      <c r="O107" t="s" s="2">
+        <v>214</v>
+      </c>
       <c r="P107" t="s" s="2">
         <v>80</v>
       </c>
@@ -14919,28 +14935,28 @@
         <v>80</v>
       </c>
       <c r="AF107" t="s" s="2">
-        <v>646</v>
+        <v>628</v>
       </c>
       <c r="AG107" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AH107" t="s" s="2">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="AI107" t="s" s="2">
         <v>102</v>
       </c>
       <c r="AJ107" t="s" s="2">
-        <v>103</v>
+        <v>146</v>
       </c>
       <c r="AK107" t="s" s="2">
-        <v>649</v>
+        <v>80</v>
       </c>
       <c r="AL107" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AM107" t="s" s="2">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="AN107" t="s" s="2">
         <v>80</v>
@@ -14951,10 +14967,10 @@
     </row>
     <row r="108" hidden="true">
       <c r="A108" t="s" s="2">
-        <v>650</v>
+        <v>651</v>
       </c>
       <c r="B108" t="s" s="2">
-        <v>650</v>
+        <v>651</v>
       </c>
       <c r="C108" s="2"/>
       <c r="D108" t="s" s="2">
@@ -14977,16 +14993,16 @@
         <v>80</v>
       </c>
       <c r="K108" t="s" s="2">
-        <v>250</v>
+        <v>179</v>
       </c>
       <c r="L108" t="s" s="2">
-        <v>651</v>
+        <v>652</v>
       </c>
       <c r="M108" t="s" s="2">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="N108" t="s" s="2">
-        <v>367</v>
+        <v>337</v>
       </c>
       <c r="O108" s="2"/>
       <c r="P108" t="s" s="2">
@@ -15012,13 +15028,13 @@
         <v>80</v>
       </c>
       <c r="X108" t="s" s="2">
-        <v>117</v>
+        <v>80</v>
       </c>
       <c r="Y108" t="s" s="2">
-        <v>653</v>
+        <v>80</v>
       </c>
       <c r="Z108" t="s" s="2">
-        <v>654</v>
+        <v>80</v>
       </c>
       <c r="AA108" t="s" s="2">
         <v>80</v>
@@ -15036,7 +15052,7 @@
         <v>80</v>
       </c>
       <c r="AF108" t="s" s="2">
-        <v>650</v>
+        <v>651</v>
       </c>
       <c r="AG108" t="s" s="2">
         <v>78</v>
@@ -15051,23 +15067,140 @@
         <v>103</v>
       </c>
       <c r="AK108" t="s" s="2">
+        <v>654</v>
+      </c>
+      <c r="AL108" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AM108" t="s" s="2">
+        <v>111</v>
+      </c>
+      <c r="AN108" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AO108" t="s" s="2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="109" hidden="true">
+      <c r="A109" t="s" s="2">
         <v>655</v>
       </c>
-      <c r="AL108" t="s" s="2">
+      <c r="B109" t="s" s="2">
+        <v>655</v>
+      </c>
+      <c r="C109" s="2"/>
+      <c r="D109" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="E109" s="2"/>
+      <c r="F109" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="G109" t="s" s="2">
+        <v>90</v>
+      </c>
+      <c r="H109" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="I109" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="J109" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="K109" t="s" s="2">
+        <v>250</v>
+      </c>
+      <c r="L109" t="s" s="2">
+        <v>656</v>
+      </c>
+      <c r="M109" t="s" s="2">
+        <v>657</v>
+      </c>
+      <c r="N109" t="s" s="2">
+        <v>367</v>
+      </c>
+      <c r="O109" s="2"/>
+      <c r="P109" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="Q109" s="2"/>
+      <c r="R109" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="S109" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="T109" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="U109" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="V109" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="W109" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="X109" t="s" s="2">
+        <v>117</v>
+      </c>
+      <c r="Y109" t="s" s="2">
+        <v>658</v>
+      </c>
+      <c r="Z109" t="s" s="2">
+        <v>659</v>
+      </c>
+      <c r="AA109" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AB109" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AC109" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AD109" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AE109" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AF109" t="s" s="2">
+        <v>655</v>
+      </c>
+      <c r="AG109" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AH109" t="s" s="2">
+        <v>90</v>
+      </c>
+      <c r="AI109" t="s" s="2">
+        <v>102</v>
+      </c>
+      <c r="AJ109" t="s" s="2">
+        <v>103</v>
+      </c>
+      <c r="AK109" t="s" s="2">
+        <v>660</v>
+      </c>
+      <c r="AL109" t="s" s="2">
         <v>371</v>
       </c>
-      <c r="AM108" t="s" s="2">
+      <c r="AM109" t="s" s="2">
         <v>372</v>
       </c>
-      <c r="AN108" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="AO108" t="s" s="2">
+      <c r="AN109" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AO109" t="s" s="2">
         <v>80</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AO108">
+  <autoFilter ref="A1:AO109">
     <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -15077,7 +15210,7 @@
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>
-  <conditionalFormatting sqref="A2:AI107">
+  <conditionalFormatting sqref="A2:AI108">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$G2&lt;&gt;"Y"</formula>
     </cfRule>

</xml_diff>